<commit_message>
fixing some formatting issues
</commit_message>
<xml_diff>
--- a/public/uploads/NUEDEXTA-2test.xlsx/graphs_NUEDEXTA-2test.xlsx
+++ b/public/uploads/NUEDEXTA-2test.xlsx/graphs_NUEDEXTA-2test.xlsx
@@ -3,9 +3,9 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <workbookPr date1904="false"/>
   <sheets>
-    <sheet name="P1 (TS) - Test P1" sheetId="1" r:id="rId4"/>
-    <sheet name="P1 NUEDEXTA User - Test P1" sheetId="2" r:id="rId5"/>
-    <sheet name="P1 Non User - Test P1" sheetId="3" r:id="rId6"/>
+    <sheet name="P1 (TS) - Test Graph" sheetId="1" r:id="rId4"/>
+    <sheet name="P1 NUEDEXTA User - Test Graph" sheetId="2" r:id="rId5"/>
+    <sheet name="P1 Non User - Test Graph" sheetId="3" r:id="rId6"/>
   </sheets>
 </workbook>
 </file>
@@ -110,7 +110,7 @@
             <c:idx val="0"/>
             <c:spPr>
               <a:solidFill>
-                <a:srgbClr val="00FF00"/>
+                <a:srgbClr val="365e92"/>
               </a:solidFill>
             </c:spPr>
           </c:dPt>
@@ -118,7 +118,7 @@
             <c:idx val="1"/>
             <c:spPr>
               <a:solidFill>
-                <a:srgbClr val="00FF00"/>
+                <a:srgbClr val="365e92"/>
               </a:solidFill>
             </c:spPr>
           </c:dPt>
@@ -126,24 +126,21 @@
             <c:idx val="2"/>
             <c:spPr>
               <a:solidFill>
-                <a:srgbClr val="00FF00"/>
+                <a:srgbClr val="365e92"/>
               </a:solidFill>
             </c:spPr>
           </c:dPt>
           <c:val>
             <c:numRef>
-              <c:f>'P1 (TS) - Test P1'!$B$4:$D$4</c:f>
+              <c:f>'P1 (TS) - Test Graph'!$B$4:$C$4</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
-                <c:ptCount val="3"/>
+                <c:ptCount val="2"/>
                 <c:pt idx="0" formatCode="General">
                   <c:v>0.07</c:v>
                 </c:pt>
                 <c:pt idx="1" formatCode="General">
                   <c:v>0.09</c:v>
-                </c:pt>
-                <c:pt idx="2" formatCode="General">
-                  <c:v>0.1</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -168,7 +165,7 @@
             <c:idx val="0"/>
             <c:spPr>
               <a:solidFill>
-                <a:srgbClr val="0000FF"/>
+                <a:srgbClr val="a5a5a5"/>
               </a:solidFill>
             </c:spPr>
           </c:dPt>
@@ -176,7 +173,7 @@
             <c:idx val="1"/>
             <c:spPr>
               <a:solidFill>
-                <a:srgbClr val="0000FF"/>
+                <a:srgbClr val="a5a5a5"/>
               </a:solidFill>
             </c:spPr>
           </c:dPt>
@@ -184,23 +181,20 @@
             <c:idx val="2"/>
             <c:spPr>
               <a:solidFill>
-                <a:srgbClr val="0000FF"/>
+                <a:srgbClr val="a5a5a5"/>
               </a:solidFill>
             </c:spPr>
           </c:dPt>
           <c:val>
             <c:numRef>
-              <c:f>'P1 (TS) - Test P1'!$B$5:$D$5</c:f>
+              <c:f>'P1 (TS) - Test Graph'!$B$5:$C$5</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
-                <c:ptCount val="3"/>
+                <c:ptCount val="2"/>
                 <c:pt idx="0" formatCode="General">
                   <c:v>0.09</c:v>
                 </c:pt>
                 <c:pt idx="1" formatCode="General">
-                  <c:v>0.1</c:v>
-                </c:pt>
-                <c:pt idx="2" formatCode="General">
                   <c:v>0.1</c:v>
                 </c:pt>
               </c:numCache>
@@ -226,7 +220,7 @@
             <c:idx val="0"/>
             <c:spPr>
               <a:solidFill>
-                <a:srgbClr val="FF0000"/>
+                <a:srgbClr val="be0712"/>
               </a:solidFill>
             </c:spPr>
           </c:dPt>
@@ -234,7 +228,7 @@
             <c:idx val="1"/>
             <c:spPr>
               <a:solidFill>
-                <a:srgbClr val="FF0000"/>
+                <a:srgbClr val="be0712"/>
               </a:solidFill>
             </c:spPr>
           </c:dPt>
@@ -242,41 +236,48 @@
             <c:idx val="2"/>
             <c:spPr>
               <a:solidFill>
-                <a:srgbClr val="FF0000"/>
+                <a:srgbClr val="be0712"/>
               </a:solidFill>
             </c:spPr>
           </c:dPt>
           <c:val>
             <c:numRef>
-              <c:f>'P1 (TS) - Test P1'!$B$6:$D$6</c:f>
+              <c:f>'P1 (TS) - Test Graph'!$B$6:$C$6</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
-                <c:ptCount val="3"/>
+                <c:ptCount val="2"/>
                 <c:pt idx="0" formatCode="General">
                   <c:v>0.84</c:v>
                 </c:pt>
                 <c:pt idx="1" formatCode="General">
                   <c:v>0.81</c:v>
-                </c:pt>
-                <c:pt idx="2" formatCode="General">
-                  <c:v>0.8</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
           </c:val>
           <c:shape val="box"/>
         </c:ser>
-        <c:axId val="7675769"/>
-        <c:axId val="15394978"/>
+        <c:axId val="15810679"/>
+        <c:axId val="9833120"/>
       </c:bar3DChart>
       <c:catAx>
-        <c:axId val="7675769"/>
+        <c:axId val="15810679"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
         <c:delete val="0"/>
         <c:axPos val="b"/>
-        <c:majorGridlines/>
+        <c:majorGridlines>
+          <c:spPr>
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+          </c:spPr>
+        </c:majorGridlines>
+        <c:title>
+          <c:layout/>
+          <c:overlay val="0"/>
+        </c:title>
         <c:numFmt formatCode="General" sourceLinked="1"/>
         <c:majorTickMark val="none"/>
         <c:minorTickMark val="none"/>
@@ -291,7 +292,7 @@
             <a:endParaRPr/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="15394978"/>
+        <c:crossAx val="9833120"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -300,13 +301,19 @@
         <c:tickMarkSkip val="1"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="15394978"/>
+        <c:axId val="9833120"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
         <c:delete val="0"/>
         <c:axPos val="b"/>
-        <c:majorGridlines/>
+        <c:majorGridlines>
+          <c:spPr>
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+          </c:spPr>
+        </c:majorGridlines>
         <c:numFmt formatCode="General" sourceLinked="1"/>
         <c:majorTickMark val="none"/>
         <c:minorTickMark val="none"/>
@@ -321,7 +328,7 @@
             <a:endParaRPr/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="7675769"/>
+        <c:crossAx val="15810679"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -389,7 +396,7 @@
             <c:idx val="0"/>
             <c:spPr>
               <a:solidFill>
-                <a:srgbClr val="00FF00"/>
+                <a:srgbClr val="365e92"/>
               </a:solidFill>
             </c:spPr>
           </c:dPt>
@@ -397,7 +404,7 @@
             <c:idx val="1"/>
             <c:spPr>
               <a:solidFill>
-                <a:srgbClr val="00FF00"/>
+                <a:srgbClr val="365e92"/>
               </a:solidFill>
             </c:spPr>
           </c:dPt>
@@ -405,23 +412,20 @@
             <c:idx val="2"/>
             <c:spPr>
               <a:solidFill>
-                <a:srgbClr val="00FF00"/>
+                <a:srgbClr val="365e92"/>
               </a:solidFill>
             </c:spPr>
           </c:dPt>
           <c:val>
             <c:numRef>
-              <c:f>'P1 NUEDEXTA User - Test P1'!$B$4:$D$4</c:f>
+              <c:f>'P1 NUEDEXTA User - Test Graph'!$B$4:$C$4</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
-                <c:ptCount val="3"/>
+                <c:ptCount val="2"/>
                 <c:pt idx="0" formatCode="General">
                   <c:v>0.07</c:v>
                 </c:pt>
                 <c:pt idx="1" formatCode="General">
-                  <c:v>0.1</c:v>
-                </c:pt>
-                <c:pt idx="2" formatCode="General">
                   <c:v>0.1</c:v>
                 </c:pt>
               </c:numCache>
@@ -447,7 +451,7 @@
             <c:idx val="0"/>
             <c:spPr>
               <a:solidFill>
-                <a:srgbClr val="0000FF"/>
+                <a:srgbClr val="a5a5a5"/>
               </a:solidFill>
             </c:spPr>
           </c:dPt>
@@ -455,7 +459,7 @@
             <c:idx val="1"/>
             <c:spPr>
               <a:solidFill>
-                <a:srgbClr val="0000FF"/>
+                <a:srgbClr val="a5a5a5"/>
               </a:solidFill>
             </c:spPr>
           </c:dPt>
@@ -463,23 +467,20 @@
             <c:idx val="2"/>
             <c:spPr>
               <a:solidFill>
-                <a:srgbClr val="0000FF"/>
+                <a:srgbClr val="a5a5a5"/>
               </a:solidFill>
             </c:spPr>
           </c:dPt>
           <c:val>
             <c:numRef>
-              <c:f>'P1 NUEDEXTA User - Test P1'!$B$5:$D$5</c:f>
+              <c:f>'P1 NUEDEXTA User - Test Graph'!$B$5:$C$5</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
-                <c:ptCount val="3"/>
+                <c:ptCount val="2"/>
                 <c:pt idx="0" formatCode="General">
                   <c:v>0.12</c:v>
                 </c:pt>
                 <c:pt idx="1" formatCode="General">
-                  <c:v>0.12</c:v>
-                </c:pt>
-                <c:pt idx="2" formatCode="General">
                   <c:v>0.12</c:v>
                 </c:pt>
               </c:numCache>
@@ -505,7 +506,7 @@
             <c:idx val="0"/>
             <c:spPr>
               <a:solidFill>
-                <a:srgbClr val="FF0000"/>
+                <a:srgbClr val="be0712"/>
               </a:solidFill>
             </c:spPr>
           </c:dPt>
@@ -513,7 +514,7 @@
             <c:idx val="1"/>
             <c:spPr>
               <a:solidFill>
-                <a:srgbClr val="FF0000"/>
+                <a:srgbClr val="be0712"/>
               </a:solidFill>
             </c:spPr>
           </c:dPt>
@@ -521,23 +522,20 @@
             <c:idx val="2"/>
             <c:spPr>
               <a:solidFill>
-                <a:srgbClr val="FF0000"/>
+                <a:srgbClr val="be0712"/>
               </a:solidFill>
             </c:spPr>
           </c:dPt>
           <c:val>
             <c:numRef>
-              <c:f>'P1 NUEDEXTA User - Test P1'!$B$6:$D$6</c:f>
+              <c:f>'P1 NUEDEXTA User - Test Graph'!$B$6:$C$6</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
-                <c:ptCount val="3"/>
+                <c:ptCount val="2"/>
                 <c:pt idx="0" formatCode="General">
                   <c:v>0.81</c:v>
                 </c:pt>
                 <c:pt idx="1" formatCode="General">
-                  <c:v>0.78</c:v>
-                </c:pt>
-                <c:pt idx="2" formatCode="General">
                   <c:v>0.78</c:v>
                 </c:pt>
               </c:numCache>
@@ -545,17 +543,38 @@
           </c:val>
           <c:shape val="box"/>
         </c:ser>
-        <c:axId val="9738407"/>
-        <c:axId val="766861"/>
+        <c:axId val="2611204"/>
+        <c:axId val="2305654"/>
       </c:bar3DChart>
       <c:catAx>
-        <c:axId val="9738407"/>
+        <c:axId val="2611204"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
         <c:delete val="0"/>
         <c:axPos val="b"/>
-        <c:majorGridlines/>
+        <c:majorGridlines>
+          <c:spPr>
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+          </c:spPr>
+        </c:majorGridlines>
+        <c:title>
+          <c:tx>
+            <c:rich>
+              <a:bodyPr/>
+              <a:lstStyle/>
+              <a:p>
+                <a:r>
+                  <a:t>NUEDEXTA User</a:t>
+                </a:r>
+              </a:p>
+            </c:rich>
+          </c:tx>
+          <c:layout/>
+          <c:overlay val="0"/>
+        </c:title>
         <c:numFmt formatCode="General" sourceLinked="1"/>
         <c:majorTickMark val="none"/>
         <c:minorTickMark val="none"/>
@@ -570,7 +589,7 @@
             <a:endParaRPr/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="766861"/>
+        <c:crossAx val="2305654"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -579,13 +598,19 @@
         <c:tickMarkSkip val="1"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="766861"/>
+        <c:axId val="2305654"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
         <c:delete val="0"/>
         <c:axPos val="b"/>
-        <c:majorGridlines/>
+        <c:majorGridlines>
+          <c:spPr>
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+          </c:spPr>
+        </c:majorGridlines>
         <c:numFmt formatCode="General" sourceLinked="1"/>
         <c:majorTickMark val="none"/>
         <c:minorTickMark val="none"/>
@@ -600,7 +625,7 @@
             <a:endParaRPr/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="9738407"/>
+        <c:crossAx val="2611204"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -668,7 +693,7 @@
             <c:idx val="0"/>
             <c:spPr>
               <a:solidFill>
-                <a:srgbClr val="00FF00"/>
+                <a:srgbClr val="365e92"/>
               </a:solidFill>
             </c:spPr>
           </c:dPt>
@@ -676,7 +701,7 @@
             <c:idx val="1"/>
             <c:spPr>
               <a:solidFill>
-                <a:srgbClr val="00FF00"/>
+                <a:srgbClr val="365e92"/>
               </a:solidFill>
             </c:spPr>
           </c:dPt>
@@ -684,24 +709,21 @@
             <c:idx val="2"/>
             <c:spPr>
               <a:solidFill>
-                <a:srgbClr val="00FF00"/>
+                <a:srgbClr val="365e92"/>
               </a:solidFill>
             </c:spPr>
           </c:dPt>
           <c:val>
             <c:numRef>
-              <c:f>'P1 Non User - Test P1'!$B$4:$D$4</c:f>
+              <c:f>'P1 Non User - Test Graph'!$B$4:$C$4</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
-                <c:ptCount val="3"/>
+                <c:ptCount val="2"/>
                 <c:pt idx="0" formatCode="General">
                   <c:v>0.07</c:v>
                 </c:pt>
                 <c:pt idx="1" formatCode="General">
                   <c:v>0.09</c:v>
-                </c:pt>
-                <c:pt idx="2" formatCode="General">
-                  <c:v>0.1</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -726,7 +748,7 @@
             <c:idx val="0"/>
             <c:spPr>
               <a:solidFill>
-                <a:srgbClr val="0000FF"/>
+                <a:srgbClr val="a5a5a5"/>
               </a:solidFill>
             </c:spPr>
           </c:dPt>
@@ -734,7 +756,7 @@
             <c:idx val="1"/>
             <c:spPr>
               <a:solidFill>
-                <a:srgbClr val="0000FF"/>
+                <a:srgbClr val="a5a5a5"/>
               </a:solidFill>
             </c:spPr>
           </c:dPt>
@@ -742,24 +764,21 @@
             <c:idx val="2"/>
             <c:spPr>
               <a:solidFill>
-                <a:srgbClr val="0000FF"/>
+                <a:srgbClr val="a5a5a5"/>
               </a:solidFill>
             </c:spPr>
           </c:dPt>
           <c:val>
             <c:numRef>
-              <c:f>'P1 Non User - Test P1'!$B$5:$D$5</c:f>
+              <c:f>'P1 Non User - Test Graph'!$B$5:$C$5</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
-                <c:ptCount val="3"/>
+                <c:ptCount val="2"/>
                 <c:pt idx="0" formatCode="General">
                   <c:v>0.07</c:v>
                 </c:pt>
                 <c:pt idx="1" formatCode="General">
                   <c:v>0.08</c:v>
-                </c:pt>
-                <c:pt idx="2" formatCode="General">
-                  <c:v>0.09</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -784,7 +803,7 @@
             <c:idx val="0"/>
             <c:spPr>
               <a:solidFill>
-                <a:srgbClr val="FF0000"/>
+                <a:srgbClr val="be0712"/>
               </a:solidFill>
             </c:spPr>
           </c:dPt>
@@ -792,7 +811,7 @@
             <c:idx val="1"/>
             <c:spPr>
               <a:solidFill>
-                <a:srgbClr val="FF0000"/>
+                <a:srgbClr val="be0712"/>
               </a:solidFill>
             </c:spPr>
           </c:dPt>
@@ -800,41 +819,59 @@
             <c:idx val="2"/>
             <c:spPr>
               <a:solidFill>
-                <a:srgbClr val="FF0000"/>
+                <a:srgbClr val="be0712"/>
               </a:solidFill>
             </c:spPr>
           </c:dPt>
           <c:val>
             <c:numRef>
-              <c:f>'P1 Non User - Test P1'!$B$6:$D$6</c:f>
+              <c:f>'P1 Non User - Test Graph'!$B$6:$C$6</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
-                <c:ptCount val="3"/>
+                <c:ptCount val="2"/>
                 <c:pt idx="0" formatCode="General">
                   <c:v>0.86</c:v>
                 </c:pt>
                 <c:pt idx="1" formatCode="General">
                   <c:v>0.83</c:v>
-                </c:pt>
-                <c:pt idx="2" formatCode="General">
-                  <c:v>0.81</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
           </c:val>
           <c:shape val="box"/>
         </c:ser>
-        <c:axId val="3106303"/>
-        <c:axId val="10283795"/>
+        <c:axId val="4628451"/>
+        <c:axId val="9851716"/>
       </c:bar3DChart>
       <c:catAx>
-        <c:axId val="3106303"/>
+        <c:axId val="4628451"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
         <c:delete val="0"/>
         <c:axPos val="b"/>
-        <c:majorGridlines/>
+        <c:majorGridlines>
+          <c:spPr>
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+          </c:spPr>
+        </c:majorGridlines>
+        <c:title>
+          <c:tx>
+            <c:rich>
+              <a:bodyPr/>
+              <a:lstStyle/>
+              <a:p>
+                <a:r>
+                  <a:t>NUEDEXTA User</a:t>
+                </a:r>
+              </a:p>
+            </c:rich>
+          </c:tx>
+          <c:layout/>
+          <c:overlay val="0"/>
+        </c:title>
         <c:numFmt formatCode="General" sourceLinked="1"/>
         <c:majorTickMark val="none"/>
         <c:minorTickMark val="none"/>
@@ -849,7 +886,7 @@
             <a:endParaRPr/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="10283795"/>
+        <c:crossAx val="9851716"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -858,13 +895,19 @@
         <c:tickMarkSkip val="1"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="10283795"/>
+        <c:axId val="9851716"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
         <c:delete val="0"/>
         <c:axPos val="b"/>
-        <c:majorGridlines/>
+        <c:majorGridlines>
+          <c:spPr>
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+          </c:spPr>
+        </c:majorGridlines>
         <c:numFmt formatCode="General" sourceLinked="1"/>
         <c:majorTickMark val="none"/>
         <c:minorTickMark val="none"/>
@@ -879,7 +922,7 @@
             <a:endParaRPr/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="3106303"/>
+        <c:crossAx val="4628451"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -1011,7 +1054,7 @@
   <sheetPr>
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:D8"/>
+  <dimension ref="A1:C8"/>
   <sheetViews>
     <sheetView windowProtection="false" tabSelected="false" showWhiteSpace="false" showOutlineSymbols="false" showFormulas="false" rightToLeft="false" showZeros="true" showRuler="true" showRowColHeaders="true" showGridLines="true" defaultGridColor="true" zoomScale="100" workbookViewId="0" zoomScaleSheetLayoutView="0" zoomScalePageLayoutView="0" zoomScaleNormal="0"/>
   </sheetViews>
@@ -1020,7 +1063,6 @@
     <col min="1" max="1" bestFit="true" customWidth="true" width="14.170786516853932"/>
     <col min="2" max="2" bestFit="true" customWidth="true" width="6.389887640449439"/>
     <col min="3" max="3" bestFit="true" customWidth="true" width="6.389887640449439"/>
-    <col min="4" max="4" bestFit="true" customWidth="true" width="6.389887640449439"/>
   </cols>
   <sheetData>
     <row r="1">
@@ -1031,7 +1073,7 @@
               <sz val="12"/>
               <b val="true"/>
             </rPr>
-            <t>Test P1</t>
+            <t>Test Graph</t>
           </r>
         </is>
       </c>
@@ -1065,11 +1107,6 @@
           <t> T2</t>
         </is>
       </c>
-      <c r="D3" s="0" t="inlineStr">
-        <is>
-          <t> T3</t>
-        </is>
-      </c>
     </row>
     <row r="4">
       <c r="A4" s="0" t="inlineStr">
@@ -1083,9 +1120,6 @@
       <c r="C4" s="0" t="n">
         <v>0.09</v>
       </c>
-      <c r="D4" s="0" t="n">
-        <v>0.1</v>
-      </c>
     </row>
     <row r="5">
       <c r="A5" s="0" t="inlineStr">
@@ -1099,9 +1133,6 @@
       <c r="C5" s="0" t="n">
         <v>0.1</v>
       </c>
-      <c r="D5" s="0" t="n">
-        <v>0.1</v>
-      </c>
     </row>
     <row r="6">
       <c r="A6" s="0" t="inlineStr">
@@ -1115,9 +1146,6 @@
       <c r="C6" s="0" t="n">
         <v>0.81</v>
       </c>
-      <c r="D6" s="0" t="n">
-        <v>0.8</v>
-      </c>
     </row>
     <row r="7">
       <c r="A7" s="0" t="inlineStr">
@@ -1131,9 +1159,6 @@
       <c r="C7" s="0" t="n">
         <v>320</v>
       </c>
-      <c r="D7" s="0" t="n">
-        <v>472</v>
-      </c>
     </row>
     <row r="8">
       <c r="A8" s="0" t="inlineStr">
@@ -1146,9 +1171,6 @@
       </c>
       <c r="C8" s="0" t="n">
         <v>320</v>
-      </c>
-      <c r="D8" s="0" t="n">
-        <v>472</v>
       </c>
     </row>
   </sheetData>
@@ -1166,16 +1188,15 @@
   <sheetPr>
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:D8"/>
+  <dimension ref="A1:C8"/>
   <sheetViews>
     <sheetView windowProtection="false" tabSelected="false" showWhiteSpace="false" showOutlineSymbols="false" showFormulas="false" rightToLeft="false" showZeros="true" showRuler="true" showRowColHeaders="true" showGridLines="true" defaultGridColor="true" zoomScale="100" workbookViewId="0" zoomScaleSheetLayoutView="0" zoomScalePageLayoutView="0" zoomScaleNormal="0"/>
   </sheetViews>
   <sheetFormatPr baseColWidth="8" defaultRowHeight="18"/>
   <cols>
-    <col min="1" max="1" bestFit="true" customWidth="true" width="28.570786516853932"/>
+    <col min="1" max="1" bestFit="true" customWidth="true" width="29.77078651685393"/>
     <col min="2" max="2" bestFit="true" customWidth="true" width="6.389887640449439"/>
     <col min="3" max="3" bestFit="true" customWidth="true" width="6.389887640449439"/>
-    <col min="4" max="4" bestFit="true" customWidth="true" width="6.389887640449439"/>
   </cols>
   <sheetData>
     <row r="1">
@@ -1186,7 +1207,7 @@
               <sz val="12"/>
               <b val="true"/>
             </rPr>
-            <t>Test P1</t>
+            <t>Test Graph</t>
           </r>
         </is>
       </c>
@@ -1199,7 +1220,7 @@
               <sz val="12"/>
               <b val="true"/>
             </rPr>
-            <t>P1 NUEDEXTA User - Test P1</t>
+            <t>P1 NUEDEXTA User - Test Graph</t>
           </r>
         </is>
       </c>
@@ -1220,11 +1241,6 @@
           <t> T2</t>
         </is>
       </c>
-      <c r="D3" s="0" t="inlineStr">
-        <is>
-          <t> T3</t>
-        </is>
-      </c>
     </row>
     <row r="4">
       <c r="A4" s="0" t="inlineStr">
@@ -1238,9 +1254,6 @@
       <c r="C4" s="0" t="n">
         <v>0.1</v>
       </c>
-      <c r="D4" s="0" t="n">
-        <v>0.1</v>
-      </c>
     </row>
     <row r="5">
       <c r="A5" s="0" t="inlineStr">
@@ -1254,9 +1267,6 @@
       <c r="C5" s="0" t="n">
         <v>0.12</v>
       </c>
-      <c r="D5" s="0" t="n">
-        <v>0.12</v>
-      </c>
     </row>
     <row r="6">
       <c r="A6" s="0" t="inlineStr">
@@ -1270,19 +1280,18 @@
       <c r="C6" s="0" t="n">
         <v>0.78</v>
       </c>
-      <c r="D6" s="0" t="n">
-        <v>0.78</v>
-      </c>
     </row>
     <row r="7">
-      <c r="A7" s="0" t="n">
+      <c r="A7" s="0" t="inlineStr">
+        <is>
+          <t>Total</t>
+        </is>
+      </c>
+      <c r="B7" s="0" t="n">
         <v>87</v>
       </c>
-      <c r="B7" s="0" t="n">
+      <c r="C7" s="0" t="n">
         <v>174</v>
-      </c>
-      <c r="C7" s="0" t="n">
-        <v>256</v>
       </c>
     </row>
     <row r="8">
@@ -1296,9 +1305,6 @@
       </c>
       <c r="C8" s="0" t="n">
         <v>146</v>
-      </c>
-      <c r="D8" s="0" t="n">
-        <v>216</v>
       </c>
     </row>
   </sheetData>
@@ -1316,16 +1322,15 @@
   <sheetPr>
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:D8"/>
+  <dimension ref="A1:C8"/>
   <sheetViews>
     <sheetView windowProtection="false" tabSelected="false" showWhiteSpace="false" showOutlineSymbols="false" showFormulas="false" rightToLeft="false" showZeros="true" showRuler="true" showRowColHeaders="true" showGridLines="true" defaultGridColor="true" zoomScale="100" workbookViewId="0" zoomScaleSheetLayoutView="0" zoomScalePageLayoutView="0" zoomScaleNormal="0"/>
   </sheetViews>
   <sheetFormatPr baseColWidth="8" defaultRowHeight="18"/>
   <cols>
-    <col min="1" max="1" bestFit="true" customWidth="true" width="22.570786516853932"/>
+    <col min="1" max="1" bestFit="true" customWidth="true" width="23.770786516853935"/>
     <col min="2" max="2" bestFit="true" customWidth="true" width="6.389887640449439"/>
     <col min="3" max="3" bestFit="true" customWidth="true" width="6.389887640449439"/>
-    <col min="4" max="4" bestFit="true" customWidth="true" width="6.389887640449439"/>
   </cols>
   <sheetData>
     <row r="1">
@@ -1336,7 +1341,7 @@
               <sz val="12"/>
               <b val="true"/>
             </rPr>
-            <t>Test P1</t>
+            <t>Test Graph</t>
           </r>
         </is>
       </c>
@@ -1349,7 +1354,7 @@
               <sz val="12"/>
               <b val="true"/>
             </rPr>
-            <t>P1 Non User - Test P1</t>
+            <t>P1 Non User - Test Graph</t>
           </r>
         </is>
       </c>
@@ -1370,11 +1375,6 @@
           <t> T2</t>
         </is>
       </c>
-      <c r="D3" s="0" t="inlineStr">
-        <is>
-          <t> T3</t>
-        </is>
-      </c>
     </row>
     <row r="4">
       <c r="A4" s="0" t="inlineStr">
@@ -1388,9 +1388,6 @@
       <c r="C4" s="0" t="n">
         <v>0.09</v>
       </c>
-      <c r="D4" s="0" t="n">
-        <v>0.1</v>
-      </c>
     </row>
     <row r="5">
       <c r="A5" s="0" t="inlineStr">
@@ -1404,9 +1401,6 @@
       <c r="C5" s="0" t="n">
         <v>0.08</v>
       </c>
-      <c r="D5" s="0" t="n">
-        <v>0.09</v>
-      </c>
     </row>
     <row r="6">
       <c r="A6" s="0" t="inlineStr">
@@ -1420,19 +1414,18 @@
       <c r="C6" s="0" t="n">
         <v>0.83</v>
       </c>
-      <c r="D6" s="0" t="n">
-        <v>0.81</v>
-      </c>
     </row>
     <row r="7">
-      <c r="A7" s="0" t="n">
+      <c r="A7" s="0" t="inlineStr">
+        <is>
+          <t>Total</t>
+        </is>
+      </c>
+      <c r="B7" s="0" t="n">
         <v>75</v>
       </c>
-      <c r="B7" s="0" t="n">
+      <c r="C7" s="0" t="n">
         <v>146</v>
-      </c>
-      <c r="C7" s="0" t="n">
-        <v>216</v>
       </c>
     </row>
     <row r="8">
@@ -1446,9 +1439,6 @@
       </c>
       <c r="C8" s="0" t="n">
         <v>174</v>
-      </c>
-      <c r="D8" s="0" t="n">
-        <v>256</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Correcting bug with spaces in filenames
</commit_message>
<xml_diff>
--- a/public/uploads/NUEDEXTA-2test.xlsx/graphs_NUEDEXTA-2test.xlsx
+++ b/public/uploads/NUEDEXTA-2test.xlsx/graphs_NUEDEXTA-2test.xlsx
@@ -257,11 +257,11 @@
           </c:val>
           <c:shape val="box"/>
         </c:ser>
-        <c:axId val="9995287"/>
-        <c:axId val="7999539"/>
+        <c:axId val="9656354"/>
+        <c:axId val="13036047"/>
       </c:bar3DChart>
       <c:catAx>
-        <c:axId val="9995287"/>
+        <c:axId val="9656354"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -275,17 +275,6 @@
           </c:spPr>
         </c:majorGridlines>
         <c:title>
-          <c:tx>
-            <c:rich>
-              <a:bodyPr/>
-              <a:lstStyle/>
-              <a:p>
-                <a:r>
-                  <a:t>["NUEDEXTA User", "Non User"]</a:t>
-                </a:r>
-              </a:p>
-            </c:rich>
-          </c:tx>
           <c:layout/>
           <c:overlay val="0"/>
         </c:title>
@@ -303,7 +292,7 @@
             <a:endParaRPr/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="7999539"/>
+        <c:crossAx val="13036047"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -312,7 +301,7 @@
         <c:tickMarkSkip val="1"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="7999539"/>
+        <c:axId val="13036047"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -339,7 +328,7 @@
             <a:endParaRPr/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="9995287"/>
+        <c:crossAx val="9656354"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -554,11 +543,11 @@
           </c:val>
           <c:shape val="box"/>
         </c:ser>
-        <c:axId val="16747845"/>
-        <c:axId val="3619557"/>
+        <c:axId val="1571841"/>
+        <c:axId val="16576314"/>
       </c:bar3DChart>
       <c:catAx>
-        <c:axId val="16747845"/>
+        <c:axId val="1571841"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -600,7 +589,7 @@
             <a:endParaRPr/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="3619557"/>
+        <c:crossAx val="16576314"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -609,7 +598,7 @@
         <c:tickMarkSkip val="1"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="3619557"/>
+        <c:axId val="16576314"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -636,7 +625,7 @@
             <a:endParaRPr/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="16747845"/>
+        <c:crossAx val="1571841"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -851,11 +840,11 @@
           </c:val>
           <c:shape val="box"/>
         </c:ser>
-        <c:axId val="12317235"/>
-        <c:axId val="5085745"/>
+        <c:axId val="38494"/>
+        <c:axId val="1416690"/>
       </c:bar3DChart>
       <c:catAx>
-        <c:axId val="12317235"/>
+        <c:axId val="38494"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -897,7 +886,7 @@
             <a:endParaRPr/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="5085745"/>
+        <c:crossAx val="1416690"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -906,7 +895,7 @@
         <c:tickMarkSkip val="1"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="5085745"/>
+        <c:axId val="1416690"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -933,7 +922,7 @@
             <a:endParaRPr/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="12317235"/>
+        <c:crossAx val="38494"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -1115,7 +1104,7 @@
       </c>
       <c r="C3" s="0" t="inlineStr">
         <is>
-          <t>T3</t>
+          <t> T2</t>
         </is>
       </c>
     </row>
@@ -1249,7 +1238,7 @@
       </c>
       <c r="C3" s="0" t="inlineStr">
         <is>
-          <t>T3</t>
+          <t> T2</t>
         </is>
       </c>
     </row>
@@ -1383,7 +1372,7 @@
       </c>
       <c r="C3" s="0" t="inlineStr">
         <is>
-          <t>T3</t>
+          <t> T2</t>
         </is>
       </c>
     </row>

</xml_diff>

<commit_message>
edit view changes, save fixes
</commit_message>
<xml_diff>
--- a/public/uploads/NUEDEXTA-2test.xlsx/graphs_NUEDEXTA-2test.xlsx
+++ b/public/uploads/NUEDEXTA-2test.xlsx/graphs_NUEDEXTA-2test.xlsx
@@ -132,15 +132,12 @@
           </c:dPt>
           <c:val>
             <c:numRef>
-              <c:f>'P1 (TS) - Test Graph'!$B$4:$C$4</c:f>
+              <c:f>'P1 (TS) - Test Graph'!$B$4:$B$4</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
-                <c:ptCount val="2"/>
+                <c:ptCount val="1"/>
                 <c:pt idx="0" formatCode="General">
                   <c:v>0.07</c:v>
-                </c:pt>
-                <c:pt idx="1" formatCode="General">
-                  <c:v>0.09</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -187,15 +184,12 @@
           </c:dPt>
           <c:val>
             <c:numRef>
-              <c:f>'P1 (TS) - Test Graph'!$B$5:$C$5</c:f>
+              <c:f>'P1 (TS) - Test Graph'!$B$5:$B$5</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
-                <c:ptCount val="2"/>
+                <c:ptCount val="1"/>
                 <c:pt idx="0" formatCode="General">
                   <c:v>0.09</c:v>
-                </c:pt>
-                <c:pt idx="1" formatCode="General">
-                  <c:v>0.1</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -242,66 +236,23 @@
           </c:dPt>
           <c:val>
             <c:numRef>
-              <c:f>'P1 (TS) - Test Graph'!$B$6:$C$6</c:f>
+              <c:f>'P1 (TS) - Test Graph'!$B$6:$B$6</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
-                <c:ptCount val="2"/>
+                <c:ptCount val="1"/>
                 <c:pt idx="0" formatCode="General">
                   <c:v>0.84</c:v>
-                </c:pt>
-                <c:pt idx="1" formatCode="General">
-                  <c:v>0.81</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
           </c:val>
           <c:shape val="box"/>
         </c:ser>
-        <c:axId val="9656354"/>
-        <c:axId val="13036047"/>
+        <c:axId val="4192278"/>
+        <c:axId val="15920863"/>
       </c:bar3DChart>
       <c:catAx>
-        <c:axId val="9656354"/>
-        <c:scaling>
-          <c:orientation val="minMax"/>
-        </c:scaling>
-        <c:delete val="0"/>
-        <c:axPos val="b"/>
-        <c:majorGridlines>
-          <c:spPr>
-            <a:ln>
-              <a:noFill/>
-            </a:ln>
-          </c:spPr>
-        </c:majorGridlines>
-        <c:title>
-          <c:layout/>
-          <c:overlay val="0"/>
-        </c:title>
-        <c:numFmt formatCode="General" sourceLinked="1"/>
-        <c:majorTickMark val="none"/>
-        <c:minorTickMark val="none"/>
-        <c:tickLblPos val="nextTo"/>
-        <c:txPr>
-          <a:bodyPr rot="0"/>
-          <a:lstStyle/>
-          <a:p>
-            <a:pPr>
-              <a:defRPr/>
-            </a:pPr>
-            <a:endParaRPr/>
-          </a:p>
-        </c:txPr>
-        <c:crossAx val="13036047"/>
-        <c:crosses val="autoZero"/>
-        <c:auto val="1"/>
-        <c:lblAlgn val="ctr"/>
-        <c:lblOffset val="100"/>
-        <c:tickLblSkip val="1"/>
-        <c:tickMarkSkip val="1"/>
-      </c:catAx>
-      <c:valAx>
-        <c:axId val="13036047"/>
+        <c:axId val="4192278"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -328,7 +279,43 @@
             <a:endParaRPr/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="9656354"/>
+        <c:crossAx val="15920863"/>
+        <c:crosses val="autoZero"/>
+        <c:auto val="1"/>
+        <c:lblAlgn val="ctr"/>
+        <c:lblOffset val="100"/>
+        <c:tickLblSkip val="1"/>
+        <c:tickMarkSkip val="1"/>
+      </c:catAx>
+      <c:valAx>
+        <c:axId val="15920863"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="b"/>
+        <c:majorGridlines>
+          <c:spPr>
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+          </c:spPr>
+        </c:majorGridlines>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:majorTickMark val="none"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:txPr>
+          <a:bodyPr rot="0"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr/>
+            </a:pPr>
+            <a:endParaRPr/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="4192278"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -418,15 +405,12 @@
           </c:dPt>
           <c:val>
             <c:numRef>
-              <c:f>'P1 NUEDEXTA User - Test Graph'!$B$4:$C$4</c:f>
+              <c:f>'P1 NUEDEXTA User - Test Graph'!$B$4:$B$4</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
-                <c:ptCount val="2"/>
+                <c:ptCount val="1"/>
                 <c:pt idx="0" formatCode="General">
                   <c:v>0.07</c:v>
-                </c:pt>
-                <c:pt idx="1" formatCode="General">
-                  <c:v>0.1</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -473,14 +457,11 @@
           </c:dPt>
           <c:val>
             <c:numRef>
-              <c:f>'P1 NUEDEXTA User - Test Graph'!$B$5:$C$5</c:f>
+              <c:f>'P1 NUEDEXTA User - Test Graph'!$B$5:$B$5</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
-                <c:ptCount val="2"/>
+                <c:ptCount val="1"/>
                 <c:pt idx="0" formatCode="General">
-                  <c:v>0.12</c:v>
-                </c:pt>
-                <c:pt idx="1" formatCode="General">
                   <c:v>0.12</c:v>
                 </c:pt>
               </c:numCache>
@@ -528,26 +509,23 @@
           </c:dPt>
           <c:val>
             <c:numRef>
-              <c:f>'P1 NUEDEXTA User - Test Graph'!$B$6:$C$6</c:f>
+              <c:f>'P1 NUEDEXTA User - Test Graph'!$B$6:$B$6</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
-                <c:ptCount val="2"/>
+                <c:ptCount val="1"/>
                 <c:pt idx="0" formatCode="General">
                   <c:v>0.81</c:v>
-                </c:pt>
-                <c:pt idx="1" formatCode="General">
-                  <c:v>0.78</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
           </c:val>
           <c:shape val="box"/>
         </c:ser>
-        <c:axId val="1571841"/>
-        <c:axId val="16576314"/>
+        <c:axId val="11668294"/>
+        <c:axId val="4296326"/>
       </c:bar3DChart>
       <c:catAx>
-        <c:axId val="1571841"/>
+        <c:axId val="11668294"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -589,7 +567,7 @@
             <a:endParaRPr/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="16576314"/>
+        <c:crossAx val="4296326"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -598,7 +576,7 @@
         <c:tickMarkSkip val="1"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="16576314"/>
+        <c:axId val="4296326"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -625,7 +603,7 @@
             <a:endParaRPr/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="1571841"/>
+        <c:crossAx val="11668294"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -715,15 +693,12 @@
           </c:dPt>
           <c:val>
             <c:numRef>
-              <c:f>'P1 Non User - Test Graph'!$B$4:$C$4</c:f>
+              <c:f>'P1 Non User - Test Graph'!$B$4:$B$4</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
-                <c:ptCount val="2"/>
+                <c:ptCount val="1"/>
                 <c:pt idx="0" formatCode="General">
                   <c:v>0.07</c:v>
-                </c:pt>
-                <c:pt idx="1" formatCode="General">
-                  <c:v>0.09</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -770,15 +745,12 @@
           </c:dPt>
           <c:val>
             <c:numRef>
-              <c:f>'P1 Non User - Test Graph'!$B$5:$C$5</c:f>
+              <c:f>'P1 Non User - Test Graph'!$B$5:$B$5</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
-                <c:ptCount val="2"/>
+                <c:ptCount val="1"/>
                 <c:pt idx="0" formatCode="General">
                   <c:v>0.07</c:v>
-                </c:pt>
-                <c:pt idx="1" formatCode="General">
-                  <c:v>0.08</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -825,26 +797,23 @@
           </c:dPt>
           <c:val>
             <c:numRef>
-              <c:f>'P1 Non User - Test Graph'!$B$6:$C$6</c:f>
+              <c:f>'P1 Non User - Test Graph'!$B$6:$B$6</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
-                <c:ptCount val="2"/>
+                <c:ptCount val="1"/>
                 <c:pt idx="0" formatCode="General">
                   <c:v>0.86</c:v>
-                </c:pt>
-                <c:pt idx="1" formatCode="General">
-                  <c:v>0.83</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
           </c:val>
           <c:shape val="box"/>
         </c:ser>
-        <c:axId val="38494"/>
-        <c:axId val="1416690"/>
+        <c:axId val="9261569"/>
+        <c:axId val="14924919"/>
       </c:bar3DChart>
       <c:catAx>
-        <c:axId val="38494"/>
+        <c:axId val="9261569"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -886,7 +855,7 @@
             <a:endParaRPr/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="1416690"/>
+        <c:crossAx val="14924919"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -895,7 +864,7 @@
         <c:tickMarkSkip val="1"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="1416690"/>
+        <c:axId val="14924919"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -922,7 +891,7 @@
             <a:endParaRPr/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="38494"/>
+        <c:crossAx val="9261569"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -1054,7 +1023,7 @@
   <sheetPr>
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:C8"/>
+  <dimension ref="A1:B8"/>
   <sheetViews>
     <sheetView windowProtection="false" tabSelected="false" showWhiteSpace="false" showOutlineSymbols="false" showFormulas="false" rightToLeft="false" showZeros="true" showRuler="true" showRowColHeaders="true" showGridLines="true" defaultGridColor="true" zoomScale="100" workbookViewId="0" zoomScaleSheetLayoutView="0" zoomScalePageLayoutView="0" zoomScaleNormal="0"/>
   </sheetViews>
@@ -1062,7 +1031,6 @@
   <cols>
     <col min="1" max="1" bestFit="true" customWidth="true" width="14.170786516853932"/>
     <col min="2" max="2" bestFit="true" customWidth="true" width="6.389887640449439"/>
-    <col min="3" max="3" bestFit="true" customWidth="true" width="6.389887640449439"/>
   </cols>
   <sheetData>
     <row r="1">
@@ -1102,11 +1070,6 @@
           <t>T1</t>
         </is>
       </c>
-      <c r="C3" s="0" t="inlineStr">
-        <is>
-          <t> T2</t>
-        </is>
-      </c>
     </row>
     <row r="4">
       <c r="A4" s="0" t="inlineStr">
@@ -1117,9 +1080,6 @@
       <c r="B4" s="0" t="n">
         <v>0.07</v>
       </c>
-      <c r="C4" s="0" t="n">
-        <v>0.09</v>
-      </c>
     </row>
     <row r="5">
       <c r="A5" s="0" t="inlineStr">
@@ -1130,9 +1090,6 @@
       <c r="B5" s="0" t="n">
         <v>0.09</v>
       </c>
-      <c r="C5" s="0" t="n">
-        <v>0.1</v>
-      </c>
     </row>
     <row r="6">
       <c r="A6" s="0" t="inlineStr">
@@ -1143,9 +1100,6 @@
       <c r="B6" s="0" t="n">
         <v>0.84</v>
       </c>
-      <c r="C6" s="0" t="n">
-        <v>0.81</v>
-      </c>
     </row>
     <row r="7">
       <c r="A7" s="0" t="inlineStr">
@@ -1156,9 +1110,6 @@
       <c r="B7" s="0" t="n">
         <v>162</v>
       </c>
-      <c r="C7" s="0" t="n">
-        <v>320</v>
-      </c>
     </row>
     <row r="8">
       <c r="A8" s="0" t="inlineStr">
@@ -1168,9 +1119,6 @@
       </c>
       <c r="B8" s="0" t="n">
         <v>162</v>
-      </c>
-      <c r="C8" s="0" t="n">
-        <v>320</v>
       </c>
     </row>
   </sheetData>
@@ -1188,7 +1136,7 @@
   <sheetPr>
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:C8"/>
+  <dimension ref="A1:B8"/>
   <sheetViews>
     <sheetView windowProtection="false" tabSelected="false" showWhiteSpace="false" showOutlineSymbols="false" showFormulas="false" rightToLeft="false" showZeros="true" showRuler="true" showRowColHeaders="true" showGridLines="true" defaultGridColor="true" zoomScale="100" workbookViewId="0" zoomScaleSheetLayoutView="0" zoomScalePageLayoutView="0" zoomScaleNormal="0"/>
   </sheetViews>
@@ -1196,7 +1144,6 @@
   <cols>
     <col min="1" max="1" bestFit="true" customWidth="true" width="29.77078651685393"/>
     <col min="2" max="2" bestFit="true" customWidth="true" width="6.389887640449439"/>
-    <col min="3" max="3" bestFit="true" customWidth="true" width="6.389887640449439"/>
   </cols>
   <sheetData>
     <row r="1">
@@ -1236,11 +1183,6 @@
           <t>T1</t>
         </is>
       </c>
-      <c r="C3" s="0" t="inlineStr">
-        <is>
-          <t> T2</t>
-        </is>
-      </c>
     </row>
     <row r="4">
       <c r="A4" s="0" t="inlineStr">
@@ -1251,9 +1193,6 @@
       <c r="B4" s="0" t="n">
         <v>0.07</v>
       </c>
-      <c r="C4" s="0" t="n">
-        <v>0.1</v>
-      </c>
     </row>
     <row r="5">
       <c r="A5" s="0" t="inlineStr">
@@ -1264,9 +1203,6 @@
       <c r="B5" s="0" t="n">
         <v>0.12</v>
       </c>
-      <c r="C5" s="0" t="n">
-        <v>0.12</v>
-      </c>
     </row>
     <row r="6">
       <c r="A6" s="0" t="inlineStr">
@@ -1277,9 +1213,6 @@
       <c r="B6" s="0" t="n">
         <v>0.81</v>
       </c>
-      <c r="C6" s="0" t="n">
-        <v>0.78</v>
-      </c>
     </row>
     <row r="7">
       <c r="A7" s="0" t="inlineStr">
@@ -1290,9 +1223,6 @@
       <c r="B7" s="0" t="n">
         <v>87</v>
       </c>
-      <c r="C7" s="0" t="n">
-        <v>174</v>
-      </c>
     </row>
     <row r="8">
       <c r="A8" s="0" t="inlineStr">
@@ -1302,9 +1232,6 @@
       </c>
       <c r="B8" s="0" t="n">
         <v>75</v>
-      </c>
-      <c r="C8" s="0" t="n">
-        <v>146</v>
       </c>
     </row>
   </sheetData>
@@ -1322,7 +1249,7 @@
   <sheetPr>
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:C8"/>
+  <dimension ref="A1:B8"/>
   <sheetViews>
     <sheetView windowProtection="false" tabSelected="false" showWhiteSpace="false" showOutlineSymbols="false" showFormulas="false" rightToLeft="false" showZeros="true" showRuler="true" showRowColHeaders="true" showGridLines="true" defaultGridColor="true" zoomScale="100" workbookViewId="0" zoomScaleSheetLayoutView="0" zoomScalePageLayoutView="0" zoomScaleNormal="0"/>
   </sheetViews>
@@ -1330,7 +1257,6 @@
   <cols>
     <col min="1" max="1" bestFit="true" customWidth="true" width="23.770786516853935"/>
     <col min="2" max="2" bestFit="true" customWidth="true" width="6.389887640449439"/>
-    <col min="3" max="3" bestFit="true" customWidth="true" width="6.389887640449439"/>
   </cols>
   <sheetData>
     <row r="1">
@@ -1370,11 +1296,6 @@
           <t>T1</t>
         </is>
       </c>
-      <c r="C3" s="0" t="inlineStr">
-        <is>
-          <t> T2</t>
-        </is>
-      </c>
     </row>
     <row r="4">
       <c r="A4" s="0" t="inlineStr">
@@ -1385,9 +1306,6 @@
       <c r="B4" s="0" t="n">
         <v>0.07</v>
       </c>
-      <c r="C4" s="0" t="n">
-        <v>0.09</v>
-      </c>
     </row>
     <row r="5">
       <c r="A5" s="0" t="inlineStr">
@@ -1398,9 +1316,6 @@
       <c r="B5" s="0" t="n">
         <v>0.07</v>
       </c>
-      <c r="C5" s="0" t="n">
-        <v>0.08</v>
-      </c>
     </row>
     <row r="6">
       <c r="A6" s="0" t="inlineStr">
@@ -1411,9 +1326,6 @@
       <c r="B6" s="0" t="n">
         <v>0.86</v>
       </c>
-      <c r="C6" s="0" t="n">
-        <v>0.83</v>
-      </c>
     </row>
     <row r="7">
       <c r="A7" s="0" t="inlineStr">
@@ -1424,9 +1336,6 @@
       <c r="B7" s="0" t="n">
         <v>75</v>
       </c>
-      <c r="C7" s="0" t="n">
-        <v>146</v>
-      </c>
     </row>
     <row r="8">
       <c r="A8" s="0" t="inlineStr">
@@ -1436,9 +1345,6 @@
       </c>
       <c r="B8" s="0" t="n">
         <v>87</v>
-      </c>
-      <c r="C8" s="0" t="n">
-        <v>174</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
adding more verbatim formatting
</commit_message>
<xml_diff>
--- a/public/uploads/NUEDEXTA-2test.xlsx/graphs_NUEDEXTA-2test.xlsx
+++ b/public/uploads/NUEDEXTA-2test.xlsx/graphs_NUEDEXTA-2test.xlsx
@@ -3,9 +3,9 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <workbookPr date1904="false"/>
   <sheets>
-    <sheet name="P1 (TS) - Test Graph" sheetId="1" r:id="rId4"/>
-    <sheet name="P1 NUEDEXTA User - Test Graph" sheetId="2" r:id="rId5"/>
-    <sheet name="P1 Non User - Test Graph" sheetId="3" r:id="rId6"/>
+    <sheet name="P1 (TS) - Test" sheetId="1" r:id="rId4"/>
+    <sheet name="P1 NUEDEXTA User - Test" sheetId="2" r:id="rId5"/>
+    <sheet name="P1 Non User - Test" sheetId="3" r:id="rId6"/>
   </sheets>
 </workbook>
 </file>
@@ -132,7 +132,7 @@
           </c:dPt>
           <c:val>
             <c:numRef>
-              <c:f>'P1 (TS) - Test Graph'!$B$4:$B$4</c:f>
+              <c:f>'P1 (TS) - Test'!$B$4:$B$4</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="1"/>
@@ -184,7 +184,7 @@
           </c:dPt>
           <c:val>
             <c:numRef>
-              <c:f>'P1 (TS) - Test Graph'!$B$5:$B$5</c:f>
+              <c:f>'P1 (TS) - Test'!$B$5:$B$5</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="1"/>
@@ -236,7 +236,7 @@
           </c:dPt>
           <c:val>
             <c:numRef>
-              <c:f>'P1 (TS) - Test Graph'!$B$6:$B$6</c:f>
+              <c:f>'P1 (TS) - Test'!$B$6:$B$6</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="1"/>
@@ -248,11 +248,11 @@
           </c:val>
           <c:shape val="box"/>
         </c:ser>
-        <c:axId val="4192278"/>
-        <c:axId val="15920863"/>
+        <c:axId val="12376170"/>
+        <c:axId val="12565413"/>
       </c:bar3DChart>
       <c:catAx>
-        <c:axId val="4192278"/>
+        <c:axId val="12376170"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -279,7 +279,7 @@
             <a:endParaRPr/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="15920863"/>
+        <c:crossAx val="12565413"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -288,7 +288,7 @@
         <c:tickMarkSkip val="1"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="15920863"/>
+        <c:axId val="12565413"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -315,7 +315,7 @@
             <a:endParaRPr/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="4192278"/>
+        <c:crossAx val="12376170"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -405,7 +405,7 @@
           </c:dPt>
           <c:val>
             <c:numRef>
-              <c:f>'P1 NUEDEXTA User - Test Graph'!$B$4:$B$4</c:f>
+              <c:f>'P1 NUEDEXTA User - Test'!$B$4:$B$4</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="1"/>
@@ -457,7 +457,7 @@
           </c:dPt>
           <c:val>
             <c:numRef>
-              <c:f>'P1 NUEDEXTA User - Test Graph'!$B$5:$B$5</c:f>
+              <c:f>'P1 NUEDEXTA User - Test'!$B$5:$B$5</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="1"/>
@@ -509,7 +509,7 @@
           </c:dPt>
           <c:val>
             <c:numRef>
-              <c:f>'P1 NUEDEXTA User - Test Graph'!$B$6:$B$6</c:f>
+              <c:f>'P1 NUEDEXTA User - Test'!$B$6:$B$6</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="1"/>
@@ -521,11 +521,11 @@
           </c:val>
           <c:shape val="box"/>
         </c:ser>
-        <c:axId val="11668294"/>
-        <c:axId val="4296326"/>
+        <c:axId val="8734535"/>
+        <c:axId val="15076812"/>
       </c:bar3DChart>
       <c:catAx>
-        <c:axId val="11668294"/>
+        <c:axId val="8734535"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -567,7 +567,7 @@
             <a:endParaRPr/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="4296326"/>
+        <c:crossAx val="15076812"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -576,7 +576,7 @@
         <c:tickMarkSkip val="1"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="4296326"/>
+        <c:axId val="15076812"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -603,7 +603,7 @@
             <a:endParaRPr/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="11668294"/>
+        <c:crossAx val="8734535"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -693,7 +693,7 @@
           </c:dPt>
           <c:val>
             <c:numRef>
-              <c:f>'P1 Non User - Test Graph'!$B$4:$B$4</c:f>
+              <c:f>'P1 Non User - Test'!$B$4:$B$4</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="1"/>
@@ -745,7 +745,7 @@
           </c:dPt>
           <c:val>
             <c:numRef>
-              <c:f>'P1 Non User - Test Graph'!$B$5:$B$5</c:f>
+              <c:f>'P1 Non User - Test'!$B$5:$B$5</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="1"/>
@@ -797,7 +797,7 @@
           </c:dPt>
           <c:val>
             <c:numRef>
-              <c:f>'P1 Non User - Test Graph'!$B$6:$B$6</c:f>
+              <c:f>'P1 Non User - Test'!$B$6:$B$6</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="1"/>
@@ -809,11 +809,11 @@
           </c:val>
           <c:shape val="box"/>
         </c:ser>
-        <c:axId val="9261569"/>
-        <c:axId val="14924919"/>
+        <c:axId val="4395994"/>
+        <c:axId val="10116601"/>
       </c:bar3DChart>
       <c:catAx>
-        <c:axId val="9261569"/>
+        <c:axId val="4395994"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -855,7 +855,7 @@
             <a:endParaRPr/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="14924919"/>
+        <c:crossAx val="10116601"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -864,7 +864,7 @@
         <c:tickMarkSkip val="1"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="14924919"/>
+        <c:axId val="10116601"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -891,7 +891,7 @@
             <a:endParaRPr/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="9261569"/>
+        <c:crossAx val="4395994"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -1041,7 +1041,7 @@
               <sz val="12"/>
               <b val="true"/>
             </rPr>
-            <t>Test Graph</t>
+            <t>Test</t>
           </r>
         </is>
       </c>
@@ -1142,7 +1142,7 @@
   </sheetViews>
   <sheetFormatPr baseColWidth="8" defaultRowHeight="18"/>
   <cols>
-    <col min="1" max="1" bestFit="true" customWidth="true" width="29.77078651685393"/>
+    <col min="1" max="1" bestFit="true" customWidth="true" width="24.97078651685393"/>
     <col min="2" max="2" bestFit="true" customWidth="true" width="6.389887640449439"/>
   </cols>
   <sheetData>
@@ -1154,7 +1154,7 @@
               <sz val="12"/>
               <b val="true"/>
             </rPr>
-            <t>Test Graph</t>
+            <t>Test</t>
           </r>
         </is>
       </c>
@@ -1167,7 +1167,7 @@
               <sz val="12"/>
               <b val="true"/>
             </rPr>
-            <t>P1 NUEDEXTA User - Test Graph</t>
+            <t>P1 NUEDEXTA User - Test</t>
           </r>
         </is>
       </c>
@@ -1255,7 +1255,7 @@
   </sheetViews>
   <sheetFormatPr baseColWidth="8" defaultRowHeight="18"/>
   <cols>
-    <col min="1" max="1" bestFit="true" customWidth="true" width="23.770786516853935"/>
+    <col min="1" max="1" bestFit="true" customWidth="true" width="18.97078651685393"/>
     <col min="2" max="2" bestFit="true" customWidth="true" width="6.389887640449439"/>
   </cols>
   <sheetData>
@@ -1267,7 +1267,7 @@
               <sz val="12"/>
               <b val="true"/>
             </rPr>
-            <t>Test Graph</t>
+            <t>Test</t>
           </r>
         </is>
       </c>
@@ -1280,7 +1280,7 @@
               <sz val="12"/>
               <b val="true"/>
             </rPr>
-            <t>P1 Non User - Test Graph</t>
+            <t>P1 Non User - Test</t>
           </r>
         </is>
       </c>

</xml_diff>

<commit_message>
adding verbatim sort logic
</commit_message>
<xml_diff>
--- a/public/uploads/NUEDEXTA-2test.xlsx/graphs_NUEDEXTA-2test.xlsx
+++ b/public/uploads/NUEDEXTA-2test.xlsx/graphs_NUEDEXTA-2test.xlsx
@@ -248,11 +248,11 @@
           </c:val>
           <c:shape val="box"/>
         </c:ser>
-        <c:axId val="12376170"/>
-        <c:axId val="12565413"/>
+        <c:axId val="2835606"/>
+        <c:axId val="15028997"/>
       </c:bar3DChart>
       <c:catAx>
-        <c:axId val="12376170"/>
+        <c:axId val="2835606"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -279,7 +279,7 @@
             <a:endParaRPr/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="12565413"/>
+        <c:crossAx val="15028997"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -288,7 +288,7 @@
         <c:tickMarkSkip val="1"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="12565413"/>
+        <c:axId val="15028997"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -315,7 +315,7 @@
             <a:endParaRPr/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="12376170"/>
+        <c:crossAx val="2835606"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -521,11 +521,11 @@
           </c:val>
           <c:shape val="box"/>
         </c:ser>
-        <c:axId val="8734535"/>
-        <c:axId val="15076812"/>
+        <c:axId val="12643621"/>
+        <c:axId val="708510"/>
       </c:bar3DChart>
       <c:catAx>
-        <c:axId val="8734535"/>
+        <c:axId val="12643621"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -567,7 +567,7 @@
             <a:endParaRPr/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="15076812"/>
+        <c:crossAx val="708510"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -576,7 +576,7 @@
         <c:tickMarkSkip val="1"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="15076812"/>
+        <c:axId val="708510"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -603,7 +603,7 @@
             <a:endParaRPr/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="8734535"/>
+        <c:crossAx val="12643621"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -809,11 +809,11 @@
           </c:val>
           <c:shape val="box"/>
         </c:ser>
-        <c:axId val="4395994"/>
-        <c:axId val="10116601"/>
+        <c:axId val="15591024"/>
+        <c:axId val="2494647"/>
       </c:bar3DChart>
       <c:catAx>
-        <c:axId val="4395994"/>
+        <c:axId val="15591024"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -855,7 +855,7 @@
             <a:endParaRPr/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="10116601"/>
+        <c:crossAx val="2494647"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -864,7 +864,7 @@
         <c:tickMarkSkip val="1"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="10116601"/>
+        <c:axId val="2494647"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -891,7 +891,7 @@
             <a:endParaRPr/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="4395994"/>
+        <c:crossAx val="15591024"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>

</xml_diff>

<commit_message>
making sure prod has latest code
</commit_message>
<xml_diff>
--- a/public/uploads/NUEDEXTA-2test.xlsx/graphs_NUEDEXTA-2test.xlsx
+++ b/public/uploads/NUEDEXTA-2test.xlsx/graphs_NUEDEXTA-2test.xlsx
@@ -248,11 +248,11 @@
           </c:val>
           <c:shape val="box"/>
         </c:ser>
-        <c:axId val="2835606"/>
-        <c:axId val="15028997"/>
+        <c:axId val="12116620"/>
+        <c:axId val="6534349"/>
       </c:bar3DChart>
       <c:catAx>
-        <c:axId val="2835606"/>
+        <c:axId val="12116620"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -279,7 +279,7 @@
             <a:endParaRPr/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="15028997"/>
+        <c:crossAx val="6534349"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -288,7 +288,7 @@
         <c:tickMarkSkip val="1"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="15028997"/>
+        <c:axId val="6534349"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -315,7 +315,7 @@
             <a:endParaRPr/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="2835606"/>
+        <c:crossAx val="12116620"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -521,11 +521,11 @@
           </c:val>
           <c:shape val="box"/>
         </c:ser>
-        <c:axId val="12643621"/>
-        <c:axId val="708510"/>
+        <c:axId val="12505887"/>
+        <c:axId val="7557016"/>
       </c:bar3DChart>
       <c:catAx>
-        <c:axId val="12643621"/>
+        <c:axId val="12505887"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -567,7 +567,7 @@
             <a:endParaRPr/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="708510"/>
+        <c:crossAx val="7557016"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -576,7 +576,7 @@
         <c:tickMarkSkip val="1"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="708510"/>
+        <c:axId val="7557016"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -603,7 +603,7 @@
             <a:endParaRPr/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="12643621"/>
+        <c:crossAx val="12505887"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -809,11 +809,11 @@
           </c:val>
           <c:shape val="box"/>
         </c:ser>
-        <c:axId val="15591024"/>
-        <c:axId val="2494647"/>
+        <c:axId val="5872233"/>
+        <c:axId val="5793891"/>
       </c:bar3DChart>
       <c:catAx>
-        <c:axId val="15591024"/>
+        <c:axId val="5872233"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -855,7 +855,7 @@
             <a:endParaRPr/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="2494647"/>
+        <c:crossAx val="5793891"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -864,7 +864,7 @@
         <c:tickMarkSkip val="1"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="2494647"/>
+        <c:axId val="5793891"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -891,7 +891,7 @@
             <a:endParaRPr/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="15591024"/>
+        <c:crossAx val="5872233"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>

</xml_diff>

<commit_message>
fixing bug with valence and s value datatypes
</commit_message>
<xml_diff>
--- a/public/uploads/NUEDEXTA-2test.xlsx/graphs_NUEDEXTA-2test.xlsx
+++ b/public/uploads/NUEDEXTA-2test.xlsx/graphs_NUEDEXTA-2test.xlsx
@@ -3,9 +3,9 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <workbookPr date1904="false"/>
   <sheets>
-    <sheet name="P1 (TS) - Test" sheetId="1" r:id="rId4"/>
-    <sheet name="P1 NUEDEXTA User - Test" sheetId="2" r:id="rId5"/>
-    <sheet name="P1 Non User - Test" sheetId="3" r:id="rId6"/>
+    <sheet name="p1 (TS) - Test" sheetId="1" r:id="rId4"/>
+    <sheet name="p1 NUEDEXTA User - Test" sheetId="2" r:id="rId5"/>
+    <sheet name="p1 Non User - Test" sheetId="3" r:id="rId6"/>
   </sheets>
 </workbook>
 </file>
@@ -132,12 +132,15 @@
           </c:dPt>
           <c:val>
             <c:numRef>
-              <c:f>'P1 (TS) - Test'!$B$4:$B$4</c:f>
+              <c:f>'p1 (TS) - Test'!$B$4:$C$4</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
-                <c:ptCount val="1"/>
+                <c:ptCount val="2"/>
                 <c:pt idx="0" formatCode="General">
                   <c:v>0.07</c:v>
+                </c:pt>
+                <c:pt idx="1" formatCode="General">
+                  <c:v>0.09</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -184,12 +187,15 @@
           </c:dPt>
           <c:val>
             <c:numRef>
-              <c:f>'P1 (TS) - Test'!$B$5:$B$5</c:f>
+              <c:f>'p1 (TS) - Test'!$B$5:$C$5</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
-                <c:ptCount val="1"/>
+                <c:ptCount val="2"/>
                 <c:pt idx="0" formatCode="General">
                   <c:v>0.09</c:v>
+                </c:pt>
+                <c:pt idx="1" formatCode="General">
+                  <c:v>0.1</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -236,23 +242,34 @@
           </c:dPt>
           <c:val>
             <c:numRef>
-              <c:f>'P1 (TS) - Test'!$B$6:$B$6</c:f>
+              <c:f>'p1 (TS) - Test'!$B$6:$C$6</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
-                <c:ptCount val="1"/>
+                <c:ptCount val="2"/>
                 <c:pt idx="0" formatCode="General">
                   <c:v>0.84</c:v>
+                </c:pt>
+                <c:pt idx="1" formatCode="General">
+                  <c:v>0.81</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
           </c:val>
           <c:shape val="box"/>
         </c:ser>
-        <c:axId val="12116620"/>
-        <c:axId val="6534349"/>
+        <c:dLbls>
+          <c:showLegendKey val="false"/>
+          <c:showVal val="true"/>
+          <c:showCatName val="false"/>
+          <c:showSerName val="false"/>
+          <c:showPercent val="true"/>
+          <c:showBubbleSize val="false"/>
+        </c:dLbls>
+        <c:axId val="16145150"/>
+        <c:axId val="16058972"/>
       </c:bar3DChart>
       <c:catAx>
-        <c:axId val="12116620"/>
+        <c:axId val="16145150"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -279,7 +296,7 @@
             <a:endParaRPr/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="6534349"/>
+        <c:crossAx val="16058972"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -288,7 +305,7 @@
         <c:tickMarkSkip val="1"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="6534349"/>
+        <c:axId val="16058972"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -315,7 +332,7 @@
             <a:endParaRPr/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="12116620"/>
+        <c:crossAx val="16145150"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -405,12 +422,15 @@
           </c:dPt>
           <c:val>
             <c:numRef>
-              <c:f>'P1 NUEDEXTA User - Test'!$B$4:$B$4</c:f>
+              <c:f>'p1 NUEDEXTA User - Test'!$B$4:$C$4</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
-                <c:ptCount val="1"/>
+                <c:ptCount val="2"/>
                 <c:pt idx="0" formatCode="General">
                   <c:v>0.07</c:v>
+                </c:pt>
+                <c:pt idx="1" formatCode="General">
+                  <c:v>0.09</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -457,12 +477,15 @@
           </c:dPt>
           <c:val>
             <c:numRef>
-              <c:f>'P1 NUEDEXTA User - Test'!$B$5:$B$5</c:f>
+              <c:f>'p1 NUEDEXTA User - Test'!$B$5:$C$5</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
-                <c:ptCount val="1"/>
+                <c:ptCount val="2"/>
                 <c:pt idx="0" formatCode="General">
-                  <c:v>0.12</c:v>
+                  <c:v>0.11</c:v>
+                </c:pt>
+                <c:pt idx="1" formatCode="General">
+                  <c:v>0.11</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -509,23 +532,26 @@
           </c:dPt>
           <c:val>
             <c:numRef>
-              <c:f>'P1 NUEDEXTA User - Test'!$B$6:$B$6</c:f>
+              <c:f>'p1 NUEDEXTA User - Test'!$B$6:$C$6</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
-                <c:ptCount val="1"/>
+                <c:ptCount val="2"/>
                 <c:pt idx="0" formatCode="General">
-                  <c:v>0.81</c:v>
+                  <c:v>0.82</c:v>
+                </c:pt>
+                <c:pt idx="1" formatCode="General">
+                  <c:v>0.79</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
           </c:val>
           <c:shape val="box"/>
         </c:ser>
-        <c:axId val="12505887"/>
-        <c:axId val="7557016"/>
+        <c:axId val="8973706"/>
+        <c:axId val="14250941"/>
       </c:bar3DChart>
       <c:catAx>
-        <c:axId val="12505887"/>
+        <c:axId val="8973706"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -567,7 +593,7 @@
             <a:endParaRPr/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="7557016"/>
+        <c:crossAx val="14250941"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -576,7 +602,7 @@
         <c:tickMarkSkip val="1"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="7557016"/>
+        <c:axId val="14250941"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -603,7 +629,7 @@
             <a:endParaRPr/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="12505887"/>
+        <c:crossAx val="8973706"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -693,12 +719,15 @@
           </c:dPt>
           <c:val>
             <c:numRef>
-              <c:f>'P1 Non User - Test'!$B$4:$B$4</c:f>
+              <c:f>'p1 Non User - Test'!$B$4:$C$4</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
-                <c:ptCount val="1"/>
+                <c:ptCount val="2"/>
                 <c:pt idx="0" formatCode="General">
-                  <c:v>0.07</c:v>
+                  <c:v>0.06</c:v>
+                </c:pt>
+                <c:pt idx="1" formatCode="General">
+                  <c:v>0.09</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -745,12 +774,15 @@
           </c:dPt>
           <c:val>
             <c:numRef>
-              <c:f>'P1 Non User - Test'!$B$5:$B$5</c:f>
+              <c:f>'p1 Non User - Test'!$B$5:$C$5</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
-                <c:ptCount val="1"/>
+                <c:ptCount val="2"/>
                 <c:pt idx="0" formatCode="General">
-                  <c:v>0.07</c:v>
+                  <c:v>0.08</c:v>
+                </c:pt>
+                <c:pt idx="1" formatCode="General">
+                  <c:v>0.08</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -797,23 +829,26 @@
           </c:dPt>
           <c:val>
             <c:numRef>
-              <c:f>'P1 Non User - Test'!$B$6:$B$6</c:f>
+              <c:f>'p1 Non User - Test'!$B$6:$C$6</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
-                <c:ptCount val="1"/>
+                <c:ptCount val="2"/>
                 <c:pt idx="0" formatCode="General">
                   <c:v>0.86</c:v>
+                </c:pt>
+                <c:pt idx="1" formatCode="General">
+                  <c:v>0.83</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
           </c:val>
           <c:shape val="box"/>
         </c:ser>
-        <c:axId val="5872233"/>
-        <c:axId val="5793891"/>
+        <c:axId val="6746806"/>
+        <c:axId val="20816"/>
       </c:bar3DChart>
       <c:catAx>
-        <c:axId val="5872233"/>
+        <c:axId val="6746806"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -855,7 +890,7 @@
             <a:endParaRPr/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="5793891"/>
+        <c:crossAx val="20816"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -864,7 +899,7 @@
         <c:tickMarkSkip val="1"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="5793891"/>
+        <c:axId val="20816"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -891,7 +926,7 @@
             <a:endParaRPr/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="5872233"/>
+        <c:crossAx val="6746806"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -1023,7 +1058,7 @@
   <sheetPr>
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:B8"/>
+  <dimension ref="A1:C8"/>
   <sheetViews>
     <sheetView windowProtection="false" tabSelected="false" showWhiteSpace="false" showOutlineSymbols="false" showFormulas="false" rightToLeft="false" showZeros="true" showRuler="true" showRowColHeaders="true" showGridLines="true" defaultGridColor="true" zoomScale="100" workbookViewId="0" zoomScaleSheetLayoutView="0" zoomScalePageLayoutView="0" zoomScaleNormal="0"/>
   </sheetViews>
@@ -1031,6 +1066,7 @@
   <cols>
     <col min="1" max="1" bestFit="true" customWidth="true" width="14.170786516853932"/>
     <col min="2" max="2" bestFit="true" customWidth="true" width="6.389887640449439"/>
+    <col min="3" max="3" bestFit="true" customWidth="true" width="6.389887640449439"/>
   </cols>
   <sheetData>
     <row r="1">
@@ -1070,6 +1106,11 @@
           <t>T1</t>
         </is>
       </c>
+      <c r="C3" s="0" t="inlineStr">
+        <is>
+          <t> T2</t>
+        </is>
+      </c>
     </row>
     <row r="4">
       <c r="A4" s="0" t="inlineStr">
@@ -1080,6 +1121,9 @@
       <c r="B4" s="0" t="n">
         <v>0.07</v>
       </c>
+      <c r="C4" s="0" t="n">
+        <v>0.09</v>
+      </c>
     </row>
     <row r="5">
       <c r="A5" s="0" t="inlineStr">
@@ -1090,6 +1134,9 @@
       <c r="B5" s="0" t="n">
         <v>0.09</v>
       </c>
+      <c r="C5" s="0" t="n">
+        <v>0.1</v>
+      </c>
     </row>
     <row r="6">
       <c r="A6" s="0" t="inlineStr">
@@ -1100,6 +1147,9 @@
       <c r="B6" s="0" t="n">
         <v>0.84</v>
       </c>
+      <c r="C6" s="0" t="n">
+        <v>0.81</v>
+      </c>
     </row>
     <row r="7">
       <c r="A7" s="0" t="inlineStr">
@@ -1108,7 +1158,10 @@
         </is>
       </c>
       <c r="B7" s="0" t="n">
-        <v>162</v>
+        <v>180</v>
+      </c>
+      <c r="C7" s="0" t="n">
+        <v>360</v>
       </c>
     </row>
     <row r="8">
@@ -1118,7 +1171,10 @@
         </is>
       </c>
       <c r="B8" s="0" t="n">
-        <v>162</v>
+        <v>180</v>
+      </c>
+      <c r="C8" s="0" t="n">
+        <v>360</v>
       </c>
     </row>
   </sheetData>
@@ -1136,7 +1192,7 @@
   <sheetPr>
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:B8"/>
+  <dimension ref="A1:C8"/>
   <sheetViews>
     <sheetView windowProtection="false" tabSelected="false" showWhiteSpace="false" showOutlineSymbols="false" showFormulas="false" rightToLeft="false" showZeros="true" showRuler="true" showRowColHeaders="true" showGridLines="true" defaultGridColor="true" zoomScale="100" workbookViewId="0" zoomScaleSheetLayoutView="0" zoomScalePageLayoutView="0" zoomScaleNormal="0"/>
   </sheetViews>
@@ -1144,6 +1200,7 @@
   <cols>
     <col min="1" max="1" bestFit="true" customWidth="true" width="24.97078651685393"/>
     <col min="2" max="2" bestFit="true" customWidth="true" width="6.389887640449439"/>
+    <col min="3" max="3" bestFit="true" customWidth="true" width="6.389887640449439"/>
   </cols>
   <sheetData>
     <row r="1">
@@ -1167,7 +1224,7 @@
               <sz val="12"/>
               <b val="true"/>
             </rPr>
-            <t>P1 NUEDEXTA User - Test</t>
+            <t>p1 NUEDEXTA User - Test</t>
           </r>
         </is>
       </c>
@@ -1183,6 +1240,11 @@
           <t>T1</t>
         </is>
       </c>
+      <c r="C3" s="0" t="inlineStr">
+        <is>
+          <t> T2</t>
+        </is>
+      </c>
     </row>
     <row r="4">
       <c r="A4" s="0" t="inlineStr">
@@ -1193,6 +1255,9 @@
       <c r="B4" s="0" t="n">
         <v>0.07</v>
       </c>
+      <c r="C4" s="0" t="n">
+        <v>0.09</v>
+      </c>
     </row>
     <row r="5">
       <c r="A5" s="0" t="inlineStr">
@@ -1201,7 +1266,10 @@
         </is>
       </c>
       <c r="B5" s="0" t="n">
-        <v>0.12</v>
+        <v>0.11</v>
+      </c>
+      <c r="C5" s="0" t="n">
+        <v>0.11</v>
       </c>
     </row>
     <row r="6">
@@ -1211,7 +1279,10 @@
         </is>
       </c>
       <c r="B6" s="0" t="n">
-        <v>0.81</v>
+        <v>0.82</v>
+      </c>
+      <c r="C6" s="0" t="n">
+        <v>0.79</v>
       </c>
     </row>
     <row r="7">
@@ -1221,7 +1292,10 @@
         </is>
       </c>
       <c r="B7" s="0" t="n">
-        <v>87</v>
+        <v>93</v>
+      </c>
+      <c r="C7" s="0" t="n">
+        <v>186</v>
       </c>
     </row>
     <row r="8">
@@ -1231,7 +1305,10 @@
         </is>
       </c>
       <c r="B8" s="0" t="n">
-        <v>75</v>
+        <v>87</v>
+      </c>
+      <c r="C8" s="0" t="n">
+        <v>174</v>
       </c>
     </row>
   </sheetData>
@@ -1249,7 +1326,7 @@
   <sheetPr>
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:B8"/>
+  <dimension ref="A1:C8"/>
   <sheetViews>
     <sheetView windowProtection="false" tabSelected="false" showWhiteSpace="false" showOutlineSymbols="false" showFormulas="false" rightToLeft="false" showZeros="true" showRuler="true" showRowColHeaders="true" showGridLines="true" defaultGridColor="true" zoomScale="100" workbookViewId="0" zoomScaleSheetLayoutView="0" zoomScalePageLayoutView="0" zoomScaleNormal="0"/>
   </sheetViews>
@@ -1257,6 +1334,7 @@
   <cols>
     <col min="1" max="1" bestFit="true" customWidth="true" width="18.97078651685393"/>
     <col min="2" max="2" bestFit="true" customWidth="true" width="6.389887640449439"/>
+    <col min="3" max="3" bestFit="true" customWidth="true" width="6.389887640449439"/>
   </cols>
   <sheetData>
     <row r="1">
@@ -1280,7 +1358,7 @@
               <sz val="12"/>
               <b val="true"/>
             </rPr>
-            <t>P1 Non User - Test</t>
+            <t>p1 Non User - Test</t>
           </r>
         </is>
       </c>
@@ -1296,6 +1374,11 @@
           <t>T1</t>
         </is>
       </c>
+      <c r="C3" s="0" t="inlineStr">
+        <is>
+          <t> T2</t>
+        </is>
+      </c>
     </row>
     <row r="4">
       <c r="A4" s="0" t="inlineStr">
@@ -1304,7 +1387,10 @@
         </is>
       </c>
       <c r="B4" s="0" t="n">
-        <v>0.07</v>
+        <v>0.06</v>
+      </c>
+      <c r="C4" s="0" t="n">
+        <v>0.09</v>
       </c>
     </row>
     <row r="5">
@@ -1314,7 +1400,10 @@
         </is>
       </c>
       <c r="B5" s="0" t="n">
-        <v>0.07</v>
+        <v>0.08</v>
+      </c>
+      <c r="C5" s="0" t="n">
+        <v>0.08</v>
       </c>
     </row>
     <row r="6">
@@ -1326,6 +1415,9 @@
       <c r="B6" s="0" t="n">
         <v>0.86</v>
       </c>
+      <c r="C6" s="0" t="n">
+        <v>0.83</v>
+      </c>
     </row>
     <row r="7">
       <c r="A7" s="0" t="inlineStr">
@@ -1334,7 +1426,10 @@
         </is>
       </c>
       <c r="B7" s="0" t="n">
-        <v>75</v>
+        <v>87</v>
+      </c>
+      <c r="C7" s="0" t="n">
+        <v>174</v>
       </c>
     </row>
     <row r="8">
@@ -1344,7 +1439,10 @@
         </is>
       </c>
       <c r="B8" s="0" t="n">
-        <v>87</v>
+        <v>93</v>
+      </c>
+      <c r="C8" s="0" t="n">
+        <v>186</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
pushing out mindset fixes and graph formatting improvements
</commit_message>
<xml_diff>
--- a/public/uploads/NUEDEXTA-2test.xlsx/graphs_NUEDEXTA-2test.xlsx
+++ b/public/uploads/NUEDEXTA-2test.xlsx/graphs_NUEDEXTA-2test.xlsx
@@ -3,20 +3,25 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <workbookPr date1904="false"/>
   <sheets>
-    <sheet name="p1 (TS) - Test" sheetId="1" r:id="rId4"/>
-    <sheet name="p1 NUEDEXTA User - Test" sheetId="2" r:id="rId5"/>
-    <sheet name="p1 Non User - Test" sheetId="3" r:id="rId6"/>
+    <sheet name="P1 (TS) - PGraphs" sheetId="1" r:id="rId4"/>
+    <sheet name="P1 NUEDEXTA User - PGraphs" sheetId="2" r:id="rId5"/>
+    <sheet name="P1 Non User - PGraphs" sheetId="3" r:id="rId6"/>
+    <sheet name="M1 (TS) - Graphs" sheetId="4" r:id="rId7"/>
+    <sheet name="M1 NUEDEXTA User - Graphs" sheetId="5" r:id="rId8"/>
+    <sheet name="M1 Non User - Graphs" sheetId="6" r:id="rId9"/>
   </sheets>
 </workbook>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <numFmts count="2">
+  <numFmts count="4">
     <numFmt numFmtId="100" formatCode="yyyy/mm/dd"/>
     <numFmt numFmtId="101" formatCode="yyyy/mm/dd hh:mm:ss"/>
+    <numFmt numFmtId="102" formatCode="0%"/>
+    <numFmt numFmtId="103" formatCode="00%"/>
   </numFmts>
-  <fonts count="2">
+  <fonts count="4">
     <font>
       <name val="Arial"/>
       <sz val="11"/>
@@ -29,6 +34,20 @@
       <b val="true"/>
       <color rgb="FF000000"/>
     </font>
+    <font>
+      <name val="Calibri"/>
+      <sz val="11"/>
+      <family val="1"/>
+      <b val="true"/>
+      <color rgb="FF000000"/>
+    </font>
+    <font>
+      <name val="Calibri"/>
+      <sz val="11"/>
+      <family val="1"/>
+      <b val="true"/>
+      <color rgb="FFFFFFFF"/>
+    </font>
   </fonts>
   <fills count="2">
     <fill>
@@ -38,7 +57,7 @@
       <patternFill patternType="gray125"/>
     </fill>
   </fills>
-  <borders count="2">
+  <borders count="3">
     <border/>
     <border>
       <left style="thin">
@@ -54,15 +73,31 @@
         <color rgb="FF000000"/>
       </bottom>
     </border>
+    <border>
+      <left style="none">
+        <color rgb="00000000"/>
+      </left>
+      <right style="none">
+        <color rgb="00000000"/>
+      </right>
+      <top style="none">
+        <color rgb="00000000"/>
+      </top>
+      <bottom style="none">
+        <color rgb="00000000"/>
+      </bottom>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf borderId="0" numFmtId="0" fontId="0" fillId="0"/>
   </cellStyleXfs>
-  <cellXfs count="4">
+  <cellXfs count="6">
     <xf borderId="0" numFmtId="0" fontId="0" fillId="0" xfId="0"/>
     <xf borderId="1" numFmtId="0" fontId="0" fillId="0" xfId="0"/>
     <xf borderId="0" numFmtId="14" fontId="0" fillId="0" xfId="0" applyNumberFormat="1"/>
-    <xf borderId="0" numFmtId="0" fontId="1" fillId="0" applyNumberFormat="false" applyFill="false" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
+    <xf borderId="0" numFmtId="102" fontId="1" fillId="0" applyNumberFormat="true" applyFill="false" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
+    <xf borderId="0" numFmtId="0" fontId="2" fillId="0" applyNumberFormat="false" applyFill="false" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
+    <xf borderId="2" numFmtId="103" fontId="3" fillId="0" applyNumberFormat="true" applyFill="false" applyFont="true" applyBorder="true" applyAlignment="false" applyProtection="false"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0"/>
@@ -78,6 +113,17 @@
   <c:style val="18"/>
   <c:chart>
     <c:title>
+      <c:tx>
+        <c:rich>
+          <a:bodyPr/>
+          <a:lstStyle/>
+          <a:p>
+            <a:r>
+              <a:t>   </a:t>
+            </a:r>
+          </a:p>
+        </c:rich>
+      </c:tx>
       <c:layout/>
       <c:overlay val="0"/>
     </c:title>
@@ -127,17 +173,31 @@
               </a:solidFill>
             </c:spPr>
           </c:dPt>
+          <c:cat>
+            <c:strRef>
+              <c:f>'P1 (TS) - PGraphs'!$B$3:$C$3</c:f>
+              <c:strCache>
+                <c:ptCount val="2"/>
+                <c:pt idx="0">
+                  <c:v>T1</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v> T2</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>'p1 (TS) - Test'!$B$4:$C$4</c:f>
+              <c:f>'P1 (TS) - PGraphs'!$B$4:$C$4</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="2"/>
                 <c:pt idx="0" formatCode="General">
-                  <c:v>7.000000000000001</c:v>
+                  <c:v>0.07</c:v>
                 </c:pt>
                 <c:pt idx="1" formatCode="General">
-                  <c:v>9.0</c:v>
+                  <c:v>0.09</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -173,15 +233,15 @@
           </c:dPt>
           <c:val>
             <c:numRef>
-              <c:f>'p1 (TS) - Test'!$B$5:$C$5</c:f>
+              <c:f>'P1 (TS) - PGraphs'!$B$5:$C$5</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="2"/>
                 <c:pt idx="0" formatCode="General">
-                  <c:v>9.0</c:v>
+                  <c:v>0.09</c:v>
                 </c:pt>
                 <c:pt idx="1" formatCode="General">
-                  <c:v>10.0</c:v>
+                  <c:v>0.1</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -217,15 +277,15 @@
           </c:dPt>
           <c:val>
             <c:numRef>
-              <c:f>'p1 (TS) - Test'!$B$6:$C$6</c:f>
+              <c:f>'P1 (TS) - PGraphs'!$B$6:$C$6</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="2"/>
                 <c:pt idx="0" formatCode="General">
-                  <c:v>84.0</c:v>
+                  <c:v>0.84</c:v>
                 </c:pt>
                 <c:pt idx="1" formatCode="General">
-                  <c:v>81.0</c:v>
+                  <c:v>0.81</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -240,11 +300,11 @@
           <c:showPercent val="true"/>
           <c:showBubbleSize val="false"/>
         </c:dLbls>
-        <c:axId val="14626878"/>
-        <c:axId val="15353686"/>
+        <c:axId val="1790548"/>
+        <c:axId val="11498641"/>
       </c:bar3DChart>
       <c:catAx>
-        <c:axId val="14626878"/>
+        <c:axId val="1790548"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -271,7 +331,7 @@
             <a:endParaRPr/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="15353686"/>
+        <c:crossAx val="11498641"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -280,19 +340,13 @@
         <c:tickMarkSkip val="1"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="15353686"/>
+        <c:axId val="11498641"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
         <c:delete val="0"/>
         <c:axPos val="b"/>
-        <c:majorGridlines>
-          <c:spPr>
-            <a:ln>
-              <a:noFill/>
-            </a:ln>
-          </c:spPr>
-        </c:majorGridlines>
+        <c:majorGridlines/>
         <c:numFmt formatCode="Percentage" sourceLinked="1"/>
         <c:majorTickMark val="none"/>
         <c:minorTickMark val="none"/>
@@ -307,7 +361,7 @@
             <a:endParaRPr/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="14626878"/>
+        <c:crossAx val="1790548"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -330,6 +384,17 @@
   <c:style val="18"/>
   <c:chart>
     <c:title>
+      <c:tx>
+        <c:rich>
+          <a:bodyPr/>
+          <a:lstStyle/>
+          <a:p>
+            <a:r>
+              <a:t>   </a:t>
+            </a:r>
+          </a:p>
+        </c:rich>
+      </c:tx>
       <c:layout/>
       <c:overlay val="0"/>
     </c:title>
@@ -355,44 +420,47 @@
         <c:ser>
           <c:idx val="0"/>
           <c:order val="0"/>
-          <c:tx>
+          <c:dPt>
+            <c:idx val="0"/>
+            <c:spPr>
+              <a:solidFill>
+                <a:srgbClr val="365e92"/>
+              </a:solidFill>
+            </c:spPr>
+          </c:dPt>
+          <c:dPt>
+            <c:idx val="1"/>
+            <c:spPr>
+              <a:solidFill>
+                <a:srgbClr val="365e92"/>
+              </a:solidFill>
+            </c:spPr>
+          </c:dPt>
+          <c:dPt>
+            <c:idx val="2"/>
+            <c:spPr>
+              <a:solidFill>
+                <a:srgbClr val="365e92"/>
+              </a:solidFill>
+            </c:spPr>
+          </c:dPt>
+          <c:cat>
             <c:strRef>
-              <c:f/>
+              <c:f>'P1 NUEDEXTA User - PGraphs'!$B$3:$C$3</c:f>
               <c:strCache>
-                <c:ptCount val="1"/>
+                <c:ptCount val="2"/>
                 <c:pt idx="0">
-                  <c:v>Positive</c:v>
+                  <c:v>T1</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v> T2</c:v>
                 </c:pt>
               </c:strCache>
             </c:strRef>
-          </c:tx>
-          <c:dPt>
-            <c:idx val="0"/>
-            <c:spPr>
-              <a:solidFill>
-                <a:srgbClr val="365e92"/>
-              </a:solidFill>
-            </c:spPr>
-          </c:dPt>
-          <c:dPt>
-            <c:idx val="1"/>
-            <c:spPr>
-              <a:solidFill>
-                <a:srgbClr val="365e92"/>
-              </a:solidFill>
-            </c:spPr>
-          </c:dPt>
-          <c:dPt>
-            <c:idx val="2"/>
-            <c:spPr>
-              <a:solidFill>
-                <a:srgbClr val="365e92"/>
-              </a:solidFill>
-            </c:spPr>
-          </c:dPt>
+          </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>'p1 NUEDEXTA User - Test'!$B$4:$C$4</c:f>
+              <c:f>'P1 NUEDEXTA User - PGraphs'!$B$4:$C$4</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="2"/>
@@ -410,17 +478,6 @@
         <c:ser>
           <c:idx val="1"/>
           <c:order val="1"/>
-          <c:tx>
-            <c:strRef>
-              <c:f/>
-              <c:strCache>
-                <c:ptCount val="1"/>
-                <c:pt idx="0">
-                  <c:v>Neutral</c:v>
-                </c:pt>
-              </c:strCache>
-            </c:strRef>
-          </c:tx>
           <c:dPt>
             <c:idx val="0"/>
             <c:spPr>
@@ -447,7 +504,7 @@
           </c:dPt>
           <c:val>
             <c:numRef>
-              <c:f>'p1 NUEDEXTA User - Test'!$B$5:$C$5</c:f>
+              <c:f>'P1 NUEDEXTA User - PGraphs'!$B$5:$C$5</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="2"/>
@@ -465,17 +522,6 @@
         <c:ser>
           <c:idx val="2"/>
           <c:order val="2"/>
-          <c:tx>
-            <c:strRef>
-              <c:f/>
-              <c:strCache>
-                <c:ptCount val="1"/>
-                <c:pt idx="0">
-                  <c:v>Negative</c:v>
-                </c:pt>
-              </c:strCache>
-            </c:strRef>
-          </c:tx>
           <c:dPt>
             <c:idx val="0"/>
             <c:spPr>
@@ -502,7 +548,7 @@
           </c:dPt>
           <c:val>
             <c:numRef>
-              <c:f>'p1 NUEDEXTA User - Test'!$B$6:$C$6</c:f>
+              <c:f>'P1 NUEDEXTA User - PGraphs'!$B$6:$C$6</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="2"/>
@@ -517,62 +563,19 @@
           </c:val>
           <c:shape val="box"/>
         </c:ser>
-        <c:axId val="11445771"/>
-        <c:axId val="14333291"/>
+        <c:dLbls>
+          <c:showLegendKey val="false"/>
+          <c:showVal val="true"/>
+          <c:showCatName val="false"/>
+          <c:showSerName val="false"/>
+          <c:showPercent val="true"/>
+          <c:showBubbleSize val="false"/>
+        </c:dLbls>
+        <c:axId val="12099187"/>
+        <c:axId val="447923"/>
       </c:bar3DChart>
       <c:catAx>
-        <c:axId val="11445771"/>
-        <c:scaling>
-          <c:orientation val="minMax"/>
-        </c:scaling>
-        <c:delete val="0"/>
-        <c:axPos val="b"/>
-        <c:majorGridlines>
-          <c:spPr>
-            <a:ln>
-              <a:noFill/>
-            </a:ln>
-          </c:spPr>
-        </c:majorGridlines>
-        <c:title>
-          <c:tx>
-            <c:rich>
-              <a:bodyPr/>
-              <a:lstStyle/>
-              <a:p>
-                <a:r>
-                  <a:t>NUEDEXTA User</a:t>
-                </a:r>
-              </a:p>
-            </c:rich>
-          </c:tx>
-          <c:layout/>
-          <c:overlay val="0"/>
-        </c:title>
-        <c:numFmt formatCode="General" sourceLinked="1"/>
-        <c:majorTickMark val="none"/>
-        <c:minorTickMark val="none"/>
-        <c:tickLblPos val="nextTo"/>
-        <c:txPr>
-          <a:bodyPr rot="0"/>
-          <a:lstStyle/>
-          <a:p>
-            <a:pPr>
-              <a:defRPr/>
-            </a:pPr>
-            <a:endParaRPr/>
-          </a:p>
-        </c:txPr>
-        <c:crossAx val="14333291"/>
-        <c:crosses val="autoZero"/>
-        <c:auto val="1"/>
-        <c:lblAlgn val="ctr"/>
-        <c:lblOffset val="100"/>
-        <c:tickLblSkip val="1"/>
-        <c:tickMarkSkip val="1"/>
-      </c:catAx>
-      <c:valAx>
-        <c:axId val="14333291"/>
+        <c:axId val="12099187"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -599,16 +602,41 @@
             <a:endParaRPr/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="11445771"/>
+        <c:crossAx val="447923"/>
+        <c:crosses val="autoZero"/>
+        <c:auto val="1"/>
+        <c:lblAlgn val="ctr"/>
+        <c:lblOffset val="100"/>
+        <c:tickLblSkip val="1"/>
+        <c:tickMarkSkip val="1"/>
+      </c:catAx>
+      <c:valAx>
+        <c:axId val="447923"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="b"/>
+        <c:majorGridlines/>
+        <c:numFmt formatCode="Percentage" sourceLinked="1"/>
+        <c:majorTickMark val="none"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:txPr>
+          <a:bodyPr rot="0"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr/>
+            </a:pPr>
+            <a:endParaRPr/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="12099187"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
     </c:plotArea>
-    <c:legend>
-      <c:legendPos val="r"/>
-      <c:layout/>
-      <c:overlay val="0"/>
-    </c:legend>
     <c:plotVisOnly val="1"/>
     <c:dispBlanksAs val="gap"/>
     <c:showDLblsOverMax val="1"/>
@@ -627,6 +655,17 @@
   <c:style val="18"/>
   <c:chart>
     <c:title>
+      <c:tx>
+        <c:rich>
+          <a:bodyPr/>
+          <a:lstStyle/>
+          <a:p>
+            <a:r>
+              <a:t>   </a:t>
+            </a:r>
+          </a:p>
+        </c:rich>
+      </c:tx>
       <c:layout/>
       <c:overlay val="0"/>
     </c:title>
@@ -652,44 +691,47 @@
         <c:ser>
           <c:idx val="0"/>
           <c:order val="0"/>
-          <c:tx>
+          <c:dPt>
+            <c:idx val="0"/>
+            <c:spPr>
+              <a:solidFill>
+                <a:srgbClr val="365e92"/>
+              </a:solidFill>
+            </c:spPr>
+          </c:dPt>
+          <c:dPt>
+            <c:idx val="1"/>
+            <c:spPr>
+              <a:solidFill>
+                <a:srgbClr val="365e92"/>
+              </a:solidFill>
+            </c:spPr>
+          </c:dPt>
+          <c:dPt>
+            <c:idx val="2"/>
+            <c:spPr>
+              <a:solidFill>
+                <a:srgbClr val="365e92"/>
+              </a:solidFill>
+            </c:spPr>
+          </c:dPt>
+          <c:cat>
             <c:strRef>
-              <c:f/>
+              <c:f>'P1 Non User - PGraphs'!$B$3:$C$3</c:f>
               <c:strCache>
-                <c:ptCount val="1"/>
+                <c:ptCount val="2"/>
                 <c:pt idx="0">
-                  <c:v>Positive</c:v>
+                  <c:v>T1</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v> T2</c:v>
                 </c:pt>
               </c:strCache>
             </c:strRef>
-          </c:tx>
-          <c:dPt>
-            <c:idx val="0"/>
-            <c:spPr>
-              <a:solidFill>
-                <a:srgbClr val="365e92"/>
-              </a:solidFill>
-            </c:spPr>
-          </c:dPt>
-          <c:dPt>
-            <c:idx val="1"/>
-            <c:spPr>
-              <a:solidFill>
-                <a:srgbClr val="365e92"/>
-              </a:solidFill>
-            </c:spPr>
-          </c:dPt>
-          <c:dPt>
-            <c:idx val="2"/>
-            <c:spPr>
-              <a:solidFill>
-                <a:srgbClr val="365e92"/>
-              </a:solidFill>
-            </c:spPr>
-          </c:dPt>
+          </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>'p1 Non User - Test'!$B$4:$C$4</c:f>
+              <c:f>'P1 Non User - PGraphs'!$B$4:$C$4</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="2"/>
@@ -707,17 +749,6 @@
         <c:ser>
           <c:idx val="1"/>
           <c:order val="1"/>
-          <c:tx>
-            <c:strRef>
-              <c:f/>
-              <c:strCache>
-                <c:ptCount val="1"/>
-                <c:pt idx="0">
-                  <c:v>Neutral</c:v>
-                </c:pt>
-              </c:strCache>
-            </c:strRef>
-          </c:tx>
           <c:dPt>
             <c:idx val="0"/>
             <c:spPr>
@@ -744,7 +775,7 @@
           </c:dPt>
           <c:val>
             <c:numRef>
-              <c:f>'p1 Non User - Test'!$B$5:$C$5</c:f>
+              <c:f>'P1 Non User - PGraphs'!$B$5:$C$5</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="2"/>
@@ -762,17 +793,6 @@
         <c:ser>
           <c:idx val="2"/>
           <c:order val="2"/>
-          <c:tx>
-            <c:strRef>
-              <c:f/>
-              <c:strCache>
-                <c:ptCount val="1"/>
-                <c:pt idx="0">
-                  <c:v>Negative</c:v>
-                </c:pt>
-              </c:strCache>
-            </c:strRef>
-          </c:tx>
           <c:dPt>
             <c:idx val="0"/>
             <c:spPr>
@@ -799,7 +819,7 @@
           </c:dPt>
           <c:val>
             <c:numRef>
-              <c:f>'p1 Non User - Test'!$B$6:$C$6</c:f>
+              <c:f>'P1 Non User - PGraphs'!$B$6:$C$6</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="2"/>
@@ -814,62 +834,19 @@
           </c:val>
           <c:shape val="box"/>
         </c:ser>
-        <c:axId val="15923881"/>
-        <c:axId val="13305677"/>
+        <c:dLbls>
+          <c:showLegendKey val="false"/>
+          <c:showVal val="true"/>
+          <c:showCatName val="false"/>
+          <c:showSerName val="false"/>
+          <c:showPercent val="true"/>
+          <c:showBubbleSize val="false"/>
+        </c:dLbls>
+        <c:axId val="14939459"/>
+        <c:axId val="14852764"/>
       </c:bar3DChart>
       <c:catAx>
-        <c:axId val="15923881"/>
-        <c:scaling>
-          <c:orientation val="minMax"/>
-        </c:scaling>
-        <c:delete val="0"/>
-        <c:axPos val="b"/>
-        <c:majorGridlines>
-          <c:spPr>
-            <a:ln>
-              <a:noFill/>
-            </a:ln>
-          </c:spPr>
-        </c:majorGridlines>
-        <c:title>
-          <c:tx>
-            <c:rich>
-              <a:bodyPr/>
-              <a:lstStyle/>
-              <a:p>
-                <a:r>
-                  <a:t>NUEDEXTA User</a:t>
-                </a:r>
-              </a:p>
-            </c:rich>
-          </c:tx>
-          <c:layout/>
-          <c:overlay val="0"/>
-        </c:title>
-        <c:numFmt formatCode="General" sourceLinked="1"/>
-        <c:majorTickMark val="none"/>
-        <c:minorTickMark val="none"/>
-        <c:tickLblPos val="nextTo"/>
-        <c:txPr>
-          <a:bodyPr rot="0"/>
-          <a:lstStyle/>
-          <a:p>
-            <a:pPr>
-              <a:defRPr/>
-            </a:pPr>
-            <a:endParaRPr/>
-          </a:p>
-        </c:txPr>
-        <c:crossAx val="13305677"/>
-        <c:crosses val="autoZero"/>
-        <c:auto val="1"/>
-        <c:lblAlgn val="ctr"/>
-        <c:lblOffset val="100"/>
-        <c:tickLblSkip val="1"/>
-        <c:tickMarkSkip val="1"/>
-      </c:catAx>
-      <c:valAx>
-        <c:axId val="13305677"/>
+        <c:axId val="14939459"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -896,16 +873,986 @@
             <a:endParaRPr/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="15923881"/>
+        <c:crossAx val="14852764"/>
+        <c:crosses val="autoZero"/>
+        <c:auto val="1"/>
+        <c:lblAlgn val="ctr"/>
+        <c:lblOffset val="100"/>
+        <c:tickLblSkip val="1"/>
+        <c:tickMarkSkip val="1"/>
+      </c:catAx>
+      <c:valAx>
+        <c:axId val="14852764"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="b"/>
+        <c:majorGridlines/>
+        <c:numFmt formatCode="Percentage" sourceLinked="1"/>
+        <c:majorTickMark val="none"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:txPr>
+          <a:bodyPr rot="0"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr/>
+            </a:pPr>
+            <a:endParaRPr/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="14939459"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
     </c:plotArea>
-    <c:legend>
-      <c:legendPos val="r"/>
+    <c:plotVisOnly val="1"/>
+    <c:dispBlanksAs val="gap"/>
+    <c:showDLblsOverMax val="1"/>
+  </c:chart>
+  <c:printSettings>
+    <c:headerFooter/>
+    <c:pageMargins b="1.0" l="0.75" r="0.75" t="1.0" header="0.5" footer="0.5"/>
+    <c:pageSetup/>
+  </c:printSettings>
+</c:chartSpace>
+</file>
+
+<file path=xl/charts/chart4.xml><?xml version="1.0" encoding="utf-8"?>
+<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <c:date1904 val="false"/>
+  <c:style val="18"/>
+  <c:chart>
+    <c:title>
+      <c:tx>
+        <c:rich>
+          <a:bodyPr/>
+          <a:lstStyle/>
+          <a:p>
+            <a:r>
+              <a:t>   </a:t>
+            </a:r>
+          </a:p>
+        </c:rich>
+      </c:tx>
       <c:layout/>
       <c:overlay val="0"/>
-    </c:legend>
+    </c:title>
+    <c:autoTitleDeleted val="false"/>
+    <c:view3D>
+      <c:rAngAx val="1"/>
+    </c:view3D>
+    <c:floor>
+      <c:thickness val="0"/>
+    </c:floor>
+    <c:sideWall>
+      <c:thickness val="0"/>
+    </c:sideWall>
+    <c:backWall>
+      <c:thickness val="0"/>
+    </c:backWall>
+    <c:plotArea>
+      <c:layout/>
+      <c:bar3DChart>
+        <c:barDir val="bar"/>
+        <c:grouping val="percentStacked"/>
+        <c:varyColors val="true"/>
+        <c:ser>
+          <c:idx val="0"/>
+          <c:order val="0"/>
+          <c:dPt>
+            <c:idx val="0"/>
+            <c:spPr>
+              <a:solidFill>
+                <a:srgbClr val="365e92"/>
+              </a:solidFill>
+            </c:spPr>
+          </c:dPt>
+          <c:dPt>
+            <c:idx val="1"/>
+            <c:spPr>
+              <a:solidFill>
+                <a:srgbClr val="365e92"/>
+              </a:solidFill>
+            </c:spPr>
+          </c:dPt>
+          <c:dPt>
+            <c:idx val="2"/>
+            <c:spPr>
+              <a:solidFill>
+                <a:srgbClr val="365e92"/>
+              </a:solidFill>
+            </c:spPr>
+          </c:dPt>
+          <c:cat>
+            <c:strRef>
+              <c:f>'M1 (TS) - Graphs'!$B$3:$C$3</c:f>
+              <c:strCache>
+                <c:ptCount val="2"/>
+                <c:pt idx="0">
+                  <c:v>T1</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v> T2</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:cat>
+          <c:val>
+            <c:numRef>
+              <c:f>'M1 (TS) - Graphs'!$B$4:$C$4</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="2"/>
+                <c:pt idx="0" formatCode="General">
+                  <c:v>0.77</c:v>
+                </c:pt>
+                <c:pt idx="1" formatCode="General">
+                  <c:v>0.74</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+          <c:shape val="box"/>
+        </c:ser>
+        <c:ser>
+          <c:idx val="1"/>
+          <c:order val="1"/>
+          <c:dPt>
+            <c:idx val="0"/>
+            <c:spPr>
+              <a:solidFill>
+                <a:srgbClr val="a5a5a5"/>
+              </a:solidFill>
+            </c:spPr>
+          </c:dPt>
+          <c:dPt>
+            <c:idx val="1"/>
+            <c:spPr>
+              <a:solidFill>
+                <a:srgbClr val="a5a5a5"/>
+              </a:solidFill>
+            </c:spPr>
+          </c:dPt>
+          <c:dPt>
+            <c:idx val="2"/>
+            <c:spPr>
+              <a:solidFill>
+                <a:srgbClr val="a5a5a5"/>
+              </a:solidFill>
+            </c:spPr>
+          </c:dPt>
+          <c:val>
+            <c:numRef>
+              <c:f>'M1 (TS) - Graphs'!$B$5:$C$5</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="2"/>
+                <c:pt idx="0" formatCode="General">
+                  <c:v>0.18</c:v>
+                </c:pt>
+                <c:pt idx="1" formatCode="General">
+                  <c:v>0.17</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+          <c:shape val="box"/>
+        </c:ser>
+        <c:ser>
+          <c:idx val="2"/>
+          <c:order val="2"/>
+          <c:dPt>
+            <c:idx val="0"/>
+            <c:spPr>
+              <a:solidFill>
+                <a:srgbClr val="ffffff"/>
+              </a:solidFill>
+            </c:spPr>
+          </c:dPt>
+          <c:dPt>
+            <c:idx val="1"/>
+            <c:spPr>
+              <a:solidFill>
+                <a:srgbClr val="ffffff"/>
+              </a:solidFill>
+            </c:spPr>
+          </c:dPt>
+          <c:dPt>
+            <c:idx val="2"/>
+            <c:spPr>
+              <a:solidFill>
+                <a:srgbClr val="ffffff"/>
+              </a:solidFill>
+            </c:spPr>
+          </c:dPt>
+          <c:val>
+            <c:numRef>
+              <c:f>'M1 (TS) - Graphs'!$B$6:$C$6</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="2"/>
+                <c:pt idx="0" formatCode="General">
+                  <c:v>0.03</c:v>
+                </c:pt>
+                <c:pt idx="1" formatCode="General">
+                  <c:v>0.06</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+          <c:shape val="box"/>
+        </c:ser>
+        <c:ser>
+          <c:idx val="3"/>
+          <c:order val="3"/>
+          <c:dPt>
+            <c:idx val="0"/>
+            <c:spPr>
+              <a:solidFill>
+                <a:srgbClr val="be0712"/>
+              </a:solidFill>
+            </c:spPr>
+          </c:dPt>
+          <c:dPt>
+            <c:idx val="1"/>
+            <c:spPr>
+              <a:solidFill>
+                <a:srgbClr val="be0712"/>
+              </a:solidFill>
+            </c:spPr>
+          </c:dPt>
+          <c:dPt>
+            <c:idx val="2"/>
+            <c:spPr>
+              <a:solidFill>
+                <a:srgbClr val="be0712"/>
+              </a:solidFill>
+            </c:spPr>
+          </c:dPt>
+          <c:val>
+            <c:numRef>
+              <c:f>'M1 (TS) - Graphs'!$B$7:$C$7</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="2"/>
+                <c:pt idx="0" formatCode="General">
+                  <c:v>0.02</c:v>
+                </c:pt>
+                <c:pt idx="1" formatCode="General">
+                  <c:v>0.03</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+          <c:shape val="box"/>
+        </c:ser>
+        <c:dLbls>
+          <c:showLegendKey val="false"/>
+          <c:showVal val="true"/>
+          <c:showCatName val="false"/>
+          <c:showSerName val="false"/>
+          <c:showPercent val="true"/>
+          <c:showBubbleSize val="false"/>
+        </c:dLbls>
+        <c:axId val="11362541"/>
+        <c:axId val="9397330"/>
+      </c:bar3DChart>
+      <c:catAx>
+        <c:axId val="11362541"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="b"/>
+        <c:majorGridlines>
+          <c:spPr>
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+          </c:spPr>
+        </c:majorGridlines>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:majorTickMark val="none"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:txPr>
+          <a:bodyPr rot="0"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr/>
+            </a:pPr>
+            <a:endParaRPr/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="9397330"/>
+        <c:crosses val="autoZero"/>
+        <c:auto val="1"/>
+        <c:lblAlgn val="ctr"/>
+        <c:lblOffset val="100"/>
+        <c:tickLblSkip val="1"/>
+        <c:tickMarkSkip val="1"/>
+      </c:catAx>
+      <c:valAx>
+        <c:axId val="9397330"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="b"/>
+        <c:majorGridlines/>
+        <c:numFmt formatCode="Percentage" sourceLinked="1"/>
+        <c:majorTickMark val="none"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:txPr>
+          <a:bodyPr rot="0"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr/>
+            </a:pPr>
+            <a:endParaRPr/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="11362541"/>
+        <c:crosses val="autoZero"/>
+        <c:crossBetween val="between"/>
+      </c:valAx>
+    </c:plotArea>
+    <c:plotVisOnly val="1"/>
+    <c:dispBlanksAs val="gap"/>
+    <c:showDLblsOverMax val="1"/>
+  </c:chart>
+  <c:printSettings>
+    <c:headerFooter/>
+    <c:pageMargins b="1.0" l="0.75" r="0.75" t="1.0" header="0.5" footer="0.5"/>
+    <c:pageSetup/>
+  </c:printSettings>
+</c:chartSpace>
+</file>
+
+<file path=xl/charts/chart5.xml><?xml version="1.0" encoding="utf-8"?>
+<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <c:date1904 val="false"/>
+  <c:style val="18"/>
+  <c:chart>
+    <c:title>
+      <c:tx>
+        <c:rich>
+          <a:bodyPr/>
+          <a:lstStyle/>
+          <a:p>
+            <a:r>
+              <a:t>   </a:t>
+            </a:r>
+          </a:p>
+        </c:rich>
+      </c:tx>
+      <c:layout/>
+      <c:overlay val="0"/>
+    </c:title>
+    <c:autoTitleDeleted val="false"/>
+    <c:view3D>
+      <c:rAngAx val="1"/>
+    </c:view3D>
+    <c:floor>
+      <c:thickness val="0"/>
+    </c:floor>
+    <c:sideWall>
+      <c:thickness val="0"/>
+    </c:sideWall>
+    <c:backWall>
+      <c:thickness val="0"/>
+    </c:backWall>
+    <c:plotArea>
+      <c:layout/>
+      <c:bar3DChart>
+        <c:barDir val="bar"/>
+        <c:grouping val="percentStacked"/>
+        <c:varyColors val="true"/>
+        <c:ser>
+          <c:idx val="0"/>
+          <c:order val="0"/>
+          <c:dPt>
+            <c:idx val="0"/>
+            <c:spPr>
+              <a:solidFill>
+                <a:srgbClr val="365e92"/>
+              </a:solidFill>
+            </c:spPr>
+          </c:dPt>
+          <c:dPt>
+            <c:idx val="1"/>
+            <c:spPr>
+              <a:solidFill>
+                <a:srgbClr val="365e92"/>
+              </a:solidFill>
+            </c:spPr>
+          </c:dPt>
+          <c:dPt>
+            <c:idx val="2"/>
+            <c:spPr>
+              <a:solidFill>
+                <a:srgbClr val="365e92"/>
+              </a:solidFill>
+            </c:spPr>
+          </c:dPt>
+          <c:cat>
+            <c:strRef>
+              <c:f>'M1 NUEDEXTA User - Graphs'!$B$3:$C$3</c:f>
+              <c:strCache>
+                <c:ptCount val="2"/>
+                <c:pt idx="0">
+                  <c:v>T1</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v> T2</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:cat>
+          <c:val>
+            <c:numRef>
+              <c:f>'M1 NUEDEXTA User - Graphs'!$B$4:$C$4</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="2"/>
+                <c:pt idx="0" formatCode="General">
+                  <c:v>0.69</c:v>
+                </c:pt>
+                <c:pt idx="1" formatCode="General">
+                  <c:v>0.67</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+          <c:shape val="box"/>
+        </c:ser>
+        <c:ser>
+          <c:idx val="1"/>
+          <c:order val="1"/>
+          <c:dPt>
+            <c:idx val="0"/>
+            <c:spPr>
+              <a:solidFill>
+                <a:srgbClr val="a5a5a5"/>
+              </a:solidFill>
+            </c:spPr>
+          </c:dPt>
+          <c:dPt>
+            <c:idx val="1"/>
+            <c:spPr>
+              <a:solidFill>
+                <a:srgbClr val="a5a5a5"/>
+              </a:solidFill>
+            </c:spPr>
+          </c:dPt>
+          <c:dPt>
+            <c:idx val="2"/>
+            <c:spPr>
+              <a:solidFill>
+                <a:srgbClr val="a5a5a5"/>
+              </a:solidFill>
+            </c:spPr>
+          </c:dPt>
+          <c:val>
+            <c:numRef>
+              <c:f>'M1 NUEDEXTA User - Graphs'!$B$5:$C$5</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="2"/>
+                <c:pt idx="0" formatCode="General">
+                  <c:v>0.24</c:v>
+                </c:pt>
+                <c:pt idx="1" formatCode="General">
+                  <c:v>0.22</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+          <c:shape val="box"/>
+        </c:ser>
+        <c:ser>
+          <c:idx val="2"/>
+          <c:order val="2"/>
+          <c:dPt>
+            <c:idx val="0"/>
+            <c:spPr>
+              <a:solidFill>
+                <a:srgbClr val="ffffff"/>
+              </a:solidFill>
+            </c:spPr>
+          </c:dPt>
+          <c:dPt>
+            <c:idx val="1"/>
+            <c:spPr>
+              <a:solidFill>
+                <a:srgbClr val="ffffff"/>
+              </a:solidFill>
+            </c:spPr>
+          </c:dPt>
+          <c:dPt>
+            <c:idx val="2"/>
+            <c:spPr>
+              <a:solidFill>
+                <a:srgbClr val="ffffff"/>
+              </a:solidFill>
+            </c:spPr>
+          </c:dPt>
+          <c:val>
+            <c:numRef>
+              <c:f>'M1 NUEDEXTA User - Graphs'!$B$6:$C$6</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="2"/>
+                <c:pt idx="0" formatCode="General">
+                  <c:v>0.07</c:v>
+                </c:pt>
+                <c:pt idx="1" formatCode="General">
+                  <c:v>0.09</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+          <c:shape val="box"/>
+        </c:ser>
+        <c:ser>
+          <c:idx val="3"/>
+          <c:order val="3"/>
+          <c:dPt>
+            <c:idx val="0"/>
+            <c:spPr>
+              <a:solidFill>
+                <a:srgbClr val="be0712"/>
+              </a:solidFill>
+            </c:spPr>
+          </c:dPt>
+          <c:dPt>
+            <c:idx val="1"/>
+            <c:spPr>
+              <a:solidFill>
+                <a:srgbClr val="be0712"/>
+              </a:solidFill>
+            </c:spPr>
+          </c:dPt>
+          <c:dPt>
+            <c:idx val="2"/>
+            <c:spPr>
+              <a:solidFill>
+                <a:srgbClr val="be0712"/>
+              </a:solidFill>
+            </c:spPr>
+          </c:dPt>
+          <c:val>
+            <c:numRef>
+              <c:f>'M1 NUEDEXTA User - Graphs'!$B$7:$C$7</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="2"/>
+                <c:pt idx="0" formatCode="General">
+                  <c:v>0.0</c:v>
+                </c:pt>
+                <c:pt idx="1" formatCode="General">
+                  <c:v>0.02</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+          <c:shape val="box"/>
+        </c:ser>
+        <c:dLbls>
+          <c:showLegendKey val="false"/>
+          <c:showVal val="true"/>
+          <c:showCatName val="false"/>
+          <c:showSerName val="false"/>
+          <c:showPercent val="true"/>
+          <c:showBubbleSize val="false"/>
+        </c:dLbls>
+        <c:axId val="2899845"/>
+        <c:axId val="9994796"/>
+      </c:bar3DChart>
+      <c:catAx>
+        <c:axId val="2899845"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="b"/>
+        <c:majorGridlines>
+          <c:spPr>
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+          </c:spPr>
+        </c:majorGridlines>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:majorTickMark val="none"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:txPr>
+          <a:bodyPr rot="0"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr/>
+            </a:pPr>
+            <a:endParaRPr/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="9994796"/>
+        <c:crosses val="autoZero"/>
+        <c:auto val="1"/>
+        <c:lblAlgn val="ctr"/>
+        <c:lblOffset val="100"/>
+        <c:tickLblSkip val="1"/>
+        <c:tickMarkSkip val="1"/>
+      </c:catAx>
+      <c:valAx>
+        <c:axId val="9994796"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="b"/>
+        <c:majorGridlines/>
+        <c:numFmt formatCode="Percentage" sourceLinked="1"/>
+        <c:majorTickMark val="none"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:txPr>
+          <a:bodyPr rot="0"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr/>
+            </a:pPr>
+            <a:endParaRPr/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="2899845"/>
+        <c:crosses val="autoZero"/>
+        <c:crossBetween val="between"/>
+      </c:valAx>
+    </c:plotArea>
+    <c:plotVisOnly val="1"/>
+    <c:dispBlanksAs val="gap"/>
+    <c:showDLblsOverMax val="1"/>
+  </c:chart>
+  <c:printSettings>
+    <c:headerFooter/>
+    <c:pageMargins b="1.0" l="0.75" r="0.75" t="1.0" header="0.5" footer="0.5"/>
+    <c:pageSetup/>
+  </c:printSettings>
+</c:chartSpace>
+</file>
+
+<file path=xl/charts/chart6.xml><?xml version="1.0" encoding="utf-8"?>
+<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <c:date1904 val="false"/>
+  <c:style val="18"/>
+  <c:chart>
+    <c:title>
+      <c:tx>
+        <c:rich>
+          <a:bodyPr/>
+          <a:lstStyle/>
+          <a:p>
+            <a:r>
+              <a:t>   </a:t>
+            </a:r>
+          </a:p>
+        </c:rich>
+      </c:tx>
+      <c:layout/>
+      <c:overlay val="0"/>
+    </c:title>
+    <c:autoTitleDeleted val="false"/>
+    <c:view3D>
+      <c:rAngAx val="1"/>
+    </c:view3D>
+    <c:floor>
+      <c:thickness val="0"/>
+    </c:floor>
+    <c:sideWall>
+      <c:thickness val="0"/>
+    </c:sideWall>
+    <c:backWall>
+      <c:thickness val="0"/>
+    </c:backWall>
+    <c:plotArea>
+      <c:layout/>
+      <c:bar3DChart>
+        <c:barDir val="bar"/>
+        <c:grouping val="percentStacked"/>
+        <c:varyColors val="true"/>
+        <c:ser>
+          <c:idx val="0"/>
+          <c:order val="0"/>
+          <c:dPt>
+            <c:idx val="0"/>
+            <c:spPr>
+              <a:solidFill>
+                <a:srgbClr val="365e92"/>
+              </a:solidFill>
+            </c:spPr>
+          </c:dPt>
+          <c:dPt>
+            <c:idx val="1"/>
+            <c:spPr>
+              <a:solidFill>
+                <a:srgbClr val="365e92"/>
+              </a:solidFill>
+            </c:spPr>
+          </c:dPt>
+          <c:dPt>
+            <c:idx val="2"/>
+            <c:spPr>
+              <a:solidFill>
+                <a:srgbClr val="365e92"/>
+              </a:solidFill>
+            </c:spPr>
+          </c:dPt>
+          <c:cat>
+            <c:strRef>
+              <c:f>'M1 Non User - Graphs'!$B$3:$C$3</c:f>
+              <c:strCache>
+                <c:ptCount val="2"/>
+                <c:pt idx="0">
+                  <c:v>T1</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v> T2</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:cat>
+          <c:val>
+            <c:numRef>
+              <c:f>'M1 Non User - Graphs'!$B$4:$C$4</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="2"/>
+                <c:pt idx="0" formatCode="General">
+                  <c:v>0.84</c:v>
+                </c:pt>
+                <c:pt idx="1" formatCode="General">
+                  <c:v>0.81</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+          <c:shape val="box"/>
+        </c:ser>
+        <c:ser>
+          <c:idx val="1"/>
+          <c:order val="1"/>
+          <c:dPt>
+            <c:idx val="0"/>
+            <c:spPr>
+              <a:solidFill>
+                <a:srgbClr val="a5a5a5"/>
+              </a:solidFill>
+            </c:spPr>
+          </c:dPt>
+          <c:dPt>
+            <c:idx val="1"/>
+            <c:spPr>
+              <a:solidFill>
+                <a:srgbClr val="a5a5a5"/>
+              </a:solidFill>
+            </c:spPr>
+          </c:dPt>
+          <c:dPt>
+            <c:idx val="2"/>
+            <c:spPr>
+              <a:solidFill>
+                <a:srgbClr val="a5a5a5"/>
+              </a:solidFill>
+            </c:spPr>
+          </c:dPt>
+          <c:val>
+            <c:numRef>
+              <c:f>'M1 Non User - Graphs'!$B$5:$C$5</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="2"/>
+                <c:pt idx="0" formatCode="General">
+                  <c:v>0.13</c:v>
+                </c:pt>
+                <c:pt idx="1" formatCode="General">
+                  <c:v>0.11</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+          <c:shape val="box"/>
+        </c:ser>
+        <c:ser>
+          <c:idx val="2"/>
+          <c:order val="2"/>
+          <c:dPt>
+            <c:idx val="0"/>
+            <c:spPr>
+              <a:solidFill>
+                <a:srgbClr val="ffffff"/>
+              </a:solidFill>
+            </c:spPr>
+          </c:dPt>
+          <c:dPt>
+            <c:idx val="1"/>
+            <c:spPr>
+              <a:solidFill>
+                <a:srgbClr val="ffffff"/>
+              </a:solidFill>
+            </c:spPr>
+          </c:dPt>
+          <c:dPt>
+            <c:idx val="2"/>
+            <c:spPr>
+              <a:solidFill>
+                <a:srgbClr val="ffffff"/>
+              </a:solidFill>
+            </c:spPr>
+          </c:dPt>
+          <c:val>
+            <c:numRef>
+              <c:f>'M1 Non User - Graphs'!$B$6:$C$6</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="2"/>
+                <c:pt idx="0" formatCode="General">
+                  <c:v>0.0</c:v>
+                </c:pt>
+                <c:pt idx="1" formatCode="General">
+                  <c:v>0.03</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+          <c:shape val="box"/>
+        </c:ser>
+        <c:ser>
+          <c:idx val="3"/>
+          <c:order val="3"/>
+          <c:dPt>
+            <c:idx val="0"/>
+            <c:spPr>
+              <a:solidFill>
+                <a:srgbClr val="be0712"/>
+              </a:solidFill>
+            </c:spPr>
+          </c:dPt>
+          <c:dPt>
+            <c:idx val="1"/>
+            <c:spPr>
+              <a:solidFill>
+                <a:srgbClr val="be0712"/>
+              </a:solidFill>
+            </c:spPr>
+          </c:dPt>
+          <c:dPt>
+            <c:idx val="2"/>
+            <c:spPr>
+              <a:solidFill>
+                <a:srgbClr val="be0712"/>
+              </a:solidFill>
+            </c:spPr>
+          </c:dPt>
+          <c:val>
+            <c:numRef>
+              <c:f>'M1 Non User - Graphs'!$B$7:$C$7</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="2"/>
+                <c:pt idx="0" formatCode="General">
+                  <c:v>0.03</c:v>
+                </c:pt>
+                <c:pt idx="1" formatCode="General">
+                  <c:v>0.05</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+          <c:shape val="box"/>
+        </c:ser>
+        <c:dLbls>
+          <c:showLegendKey val="false"/>
+          <c:showVal val="true"/>
+          <c:showCatName val="false"/>
+          <c:showSerName val="false"/>
+          <c:showPercent val="true"/>
+          <c:showBubbleSize val="false"/>
+        </c:dLbls>
+        <c:axId val="1332701"/>
+        <c:axId val="2462853"/>
+      </c:bar3DChart>
+      <c:catAx>
+        <c:axId val="1332701"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="b"/>
+        <c:majorGridlines>
+          <c:spPr>
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+          </c:spPr>
+        </c:majorGridlines>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:majorTickMark val="none"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:txPr>
+          <a:bodyPr rot="0"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr/>
+            </a:pPr>
+            <a:endParaRPr/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="2462853"/>
+        <c:crosses val="autoZero"/>
+        <c:auto val="1"/>
+        <c:lblAlgn val="ctr"/>
+        <c:lblOffset val="100"/>
+        <c:tickLblSkip val="1"/>
+        <c:tickMarkSkip val="1"/>
+      </c:catAx>
+      <c:valAx>
+        <c:axId val="2462853"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="b"/>
+        <c:majorGridlines/>
+        <c:numFmt formatCode="Percentage" sourceLinked="1"/>
+        <c:majorTickMark val="none"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:txPr>
+          <a:bodyPr rot="0"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr/>
+            </a:pPr>
+            <a:endParaRPr/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="1332701"/>
+        <c:crosses val="autoZero"/>
+        <c:crossBetween val="between"/>
+      </c:valAx>
+    </c:plotArea>
     <c:plotVisOnly val="1"/>
     <c:dispBlanksAs val="gap"/>
     <c:showDLblsOverMax val="1"/>
@@ -944,7 +1891,7 @@
       </xdr:xfrm>
       <a:graphic>
         <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
-          <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId20"/>
+          <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId53"/>
         </a:graphicData>
       </a:graphic>
     </xdr:graphicFrame>
@@ -957,15 +1904,15 @@
 <xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
   <xdr:twoCellAnchor>
     <xdr:from>
-      <xdr:col>3</xdr:col>
+      <xdr:col>1</xdr:col>
       <xdr:colOff>0</xdr:colOff>
-      <xdr:row>8</xdr:row>
+      <xdr:row>9</xdr:row>
       <xdr:rowOff>0</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>7</xdr:col>
+      <xdr:col>14</xdr:col>
       <xdr:colOff>0</xdr:colOff>
-      <xdr:row>20</xdr:row>
+      <xdr:row>31</xdr:row>
       <xdr:rowOff>0</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame>
@@ -979,7 +1926,7 @@
       </xdr:xfrm>
       <a:graphic>
         <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
-          <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId22"/>
+          <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId55"/>
         </a:graphicData>
       </a:graphic>
     </xdr:graphicFrame>
@@ -992,15 +1939,15 @@
 <xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
   <xdr:twoCellAnchor>
     <xdr:from>
-      <xdr:col>3</xdr:col>
+      <xdr:col>1</xdr:col>
       <xdr:colOff>0</xdr:colOff>
-      <xdr:row>8</xdr:row>
+      <xdr:row>9</xdr:row>
       <xdr:rowOff>0</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>7</xdr:col>
+      <xdr:col>14</xdr:col>
       <xdr:colOff>0</xdr:colOff>
-      <xdr:row>20</xdr:row>
+      <xdr:row>31</xdr:row>
       <xdr:rowOff>0</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame>
@@ -1014,7 +1961,112 @@
       </xdr:xfrm>
       <a:graphic>
         <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
-          <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId24"/>
+          <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId57"/>
+        </a:graphicData>
+      </a:graphic>
+    </xdr:graphicFrame>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+</xdr:wsDr>
+</file>
+
+<file path=xl/drawings/drawing4.xml><?xml version="1.0" encoding="utf-8"?>
+<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>1</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
+      <xdr:row>9</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>14</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
+      <xdr:row>31</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:to>
+    <xdr:graphicFrame>
+      <xdr:nvGraphicFramePr>
+        <xdr:cNvPr id="3" name="item_3"/>
+        <xdr:cNvGraphicFramePr/>
+      </xdr:nvGraphicFramePr>
+      <xdr:xfrm>
+        <a:off x="0" y="0"/>
+        <a:ext cx="0" cy="0"/>
+      </xdr:xfrm>
+      <a:graphic>
+        <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
+          <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId59"/>
+        </a:graphicData>
+      </a:graphic>
+    </xdr:graphicFrame>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+</xdr:wsDr>
+</file>
+
+<file path=xl/drawings/drawing5.xml><?xml version="1.0" encoding="utf-8"?>
+<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>1</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
+      <xdr:row>9</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>14</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
+      <xdr:row>31</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:to>
+    <xdr:graphicFrame>
+      <xdr:nvGraphicFramePr>
+        <xdr:cNvPr id="4" name="item_4"/>
+        <xdr:cNvGraphicFramePr/>
+      </xdr:nvGraphicFramePr>
+      <xdr:xfrm>
+        <a:off x="0" y="0"/>
+        <a:ext cx="0" cy="0"/>
+      </xdr:xfrm>
+      <a:graphic>
+        <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
+          <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId61"/>
+        </a:graphicData>
+      </a:graphic>
+    </xdr:graphicFrame>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+</xdr:wsDr>
+</file>
+
+<file path=xl/drawings/drawing6.xml><?xml version="1.0" encoding="utf-8"?>
+<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>1</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
+      <xdr:row>9</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>14</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
+      <xdr:row>31</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:to>
+    <xdr:graphicFrame>
+      <xdr:nvGraphicFramePr>
+        <xdr:cNvPr id="5" name="item_5"/>
+        <xdr:cNvGraphicFramePr/>
+      </xdr:nvGraphicFramePr>
+      <xdr:xfrm>
+        <a:off x="0" y="0"/>
+        <a:ext cx="0" cy="0"/>
+      </xdr:xfrm>
+      <a:graphic>
+        <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
+          <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId63"/>
         </a:graphicData>
       </a:graphic>
     </xdr:graphicFrame>
@@ -1035,7 +2087,7 @@
   <sheetFormatPr baseColWidth="8" defaultRowHeight="18"/>
   <cols>
     <col min="1" max="1" bestFit="true" customWidth="true" width="17.834831460674156"/>
-    <col min="2" max="2" bestFit="true" customWidth="true" width="31.034831460674155"/>
+    <col min="2" max="2" bestFit="true" customWidth="true" width="9.584831460674158"/>
     <col min="3" max="3" bestFit="true" customWidth="true" width="9.584831460674158"/>
   </cols>
   <sheetData>
@@ -1048,7 +2100,7 @@
               <rFont val="Calibri"/>
               <b val="true"/>
             </rPr>
-            <t>Test</t>
+            <t>PGraphs</t>
           </r>
         </is>
       </c>
@@ -1091,10 +2143,10 @@
         </is>
       </c>
       <c r="B4" s="3" t="n">
-        <v>7.000000000000001</v>
+        <v>0.07</v>
       </c>
       <c r="C4" s="3" t="n">
-        <v>9.0</v>
+        <v>0.09</v>
       </c>
     </row>
     <row r="5">
@@ -1104,10 +2156,10 @@
         </is>
       </c>
       <c r="B5" s="3" t="n">
-        <v>9.0</v>
+        <v>0.09</v>
       </c>
       <c r="C5" s="3" t="n">
-        <v>10.0</v>
+        <v>0.1</v>
       </c>
     </row>
     <row r="6">
@@ -1117,35 +2169,35 @@
         </is>
       </c>
       <c r="B6" s="3" t="n">
-        <v>84.0</v>
+        <v>0.84</v>
       </c>
       <c r="C6" s="3" t="n">
-        <v>81.0</v>
+        <v>0.81</v>
       </c>
     </row>
     <row r="7">
-      <c r="A7" s="3" t="inlineStr">
+      <c r="A7" s="4" t="inlineStr">
         <is>
           <t>Total</t>
         </is>
       </c>
-      <c r="B7" s="3" t="n">
+      <c r="B7" s="4" t="n">
         <v>180</v>
       </c>
-      <c r="C7" s="3" t="n">
+      <c r="C7" s="4" t="n">
         <v>360</v>
       </c>
     </row>
     <row r="8">
-      <c r="A8" s="3" t="inlineStr">
+      <c r="A8" s="4" t="inlineStr">
         <is>
           <t>Message Index</t>
         </is>
       </c>
-      <c r="B8" s="3" t="n">
+      <c r="B8" s="4" t="n">
         <v>180</v>
       </c>
-      <c r="C8" s="3" t="n">
+      <c r="C8" s="4" t="n">
         <v>360</v>
       </c>
     </row>
@@ -1155,7 +2207,7 @@
   <pageMargins right="0.75" left="0.75" bottom="1.0" top="1.0" footer="0.5" header="0.5"/>
   <pageSetup/>
   <headerFooter/>
-  <drawing r:id="rId26"/>
+  <drawing r:id="rId65"/>
 </worksheet>
 </file>
 
@@ -1170,9 +2222,9 @@
   </sheetViews>
   <sheetFormatPr baseColWidth="8" defaultRowHeight="18"/>
   <cols>
-    <col min="1" max="1" bestFit="true" customWidth="true" width="24.97078651685393"/>
-    <col min="2" max="2" bestFit="true" customWidth="true" width="6.389887640449439"/>
-    <col min="3" max="3" bestFit="true" customWidth="true" width="6.389887640449439"/>
+    <col min="1" max="1" bestFit="true" customWidth="true" width="27.370786516853933"/>
+    <col min="2" max="2" bestFit="true" customWidth="true" width="9.584831460674158"/>
+    <col min="3" max="3" bestFit="true" customWidth="true" width="9.584831460674158"/>
   </cols>
   <sheetData>
     <row r="1">
@@ -1183,7 +2235,7 @@
               <sz val="12"/>
               <b val="true"/>
             </rPr>
-            <t>Test</t>
+            <t>PGraphs</t>
           </r>
         </is>
       </c>
@@ -1196,7 +2248,7 @@
               <sz val="12"/>
               <b val="true"/>
             </rPr>
-            <t>p1 NUEDEXTA User - Test</t>
+            <t>P1 NUEDEXTA User - PGraphs</t>
           </r>
         </is>
       </c>
@@ -1219,67 +2271,67 @@
       </c>
     </row>
     <row r="4">
-      <c r="A4" s="0" t="inlineStr">
+      <c r="A4" s="3" t="inlineStr">
         <is>
           <t>Positive</t>
         </is>
       </c>
-      <c r="B4" s="0" t="n">
+      <c r="B4" s="3" t="n">
         <v>0.07</v>
       </c>
-      <c r="C4" s="0" t="n">
+      <c r="C4" s="3" t="n">
         <v>0.09</v>
       </c>
     </row>
     <row r="5">
-      <c r="A5" s="0" t="inlineStr">
+      <c r="A5" s="3" t="inlineStr">
         <is>
           <t>Neutral</t>
         </is>
       </c>
-      <c r="B5" s="0" t="n">
+      <c r="B5" s="3" t="n">
         <v>0.11</v>
       </c>
-      <c r="C5" s="0" t="n">
+      <c r="C5" s="3" t="n">
         <v>0.11</v>
       </c>
     </row>
     <row r="6">
-      <c r="A6" s="0" t="inlineStr">
+      <c r="A6" s="3" t="inlineStr">
         <is>
           <t>Negative</t>
         </is>
       </c>
-      <c r="B6" s="0" t="n">
+      <c r="B6" s="3" t="n">
         <v>0.82</v>
       </c>
-      <c r="C6" s="0" t="n">
+      <c r="C6" s="3" t="n">
         <v>0.79</v>
       </c>
     </row>
     <row r="7">
-      <c r="A7" s="0" t="inlineStr">
+      <c r="A7" s="4" t="inlineStr">
         <is>
           <t>Total</t>
         </is>
       </c>
-      <c r="B7" s="0" t="n">
+      <c r="B7" s="4" t="n">
         <v>93</v>
       </c>
-      <c r="C7" s="0" t="n">
+      <c r="C7" s="4" t="n">
         <v>186</v>
       </c>
     </row>
     <row r="8">
-      <c r="A8" s="0" t="inlineStr">
+      <c r="A8" s="4" t="inlineStr">
         <is>
           <t>Message Index</t>
         </is>
       </c>
-      <c r="B8" s="0" t="n">
+      <c r="B8" s="4" t="n">
         <v>87</v>
       </c>
-      <c r="C8" s="0" t="n">
+      <c r="C8" s="4" t="n">
         <v>174</v>
       </c>
     </row>
@@ -1289,7 +2341,7 @@
   <pageMargins right="0.75" left="0.75" bottom="1.0" top="1.0" footer="0.5" header="0.5"/>
   <pageSetup/>
   <headerFooter/>
-  <drawing r:id="rId28"/>
+  <drawing r:id="rId67"/>
 </worksheet>
 </file>
 
@@ -1304,9 +2356,9 @@
   </sheetViews>
   <sheetFormatPr baseColWidth="8" defaultRowHeight="18"/>
   <cols>
-    <col min="1" max="1" bestFit="true" customWidth="true" width="18.97078651685393"/>
-    <col min="2" max="2" bestFit="true" customWidth="true" width="6.389887640449439"/>
-    <col min="3" max="3" bestFit="true" customWidth="true" width="6.389887640449439"/>
+    <col min="1" max="1" bestFit="true" customWidth="true" width="21.370786516853933"/>
+    <col min="2" max="2" bestFit="true" customWidth="true" width="9.584831460674158"/>
+    <col min="3" max="3" bestFit="true" customWidth="true" width="9.584831460674158"/>
   </cols>
   <sheetData>
     <row r="1">
@@ -1317,7 +2369,7 @@
               <sz val="12"/>
               <b val="true"/>
             </rPr>
-            <t>Test</t>
+            <t>PGraphs</t>
           </r>
         </is>
       </c>
@@ -1330,7 +2382,7 @@
               <sz val="12"/>
               <b val="true"/>
             </rPr>
-            <t>p1 Non User - Test</t>
+            <t>P1 Non User - PGraphs</t>
           </r>
         </is>
       </c>
@@ -1353,67 +2405,67 @@
       </c>
     </row>
     <row r="4">
-      <c r="A4" s="0" t="inlineStr">
+      <c r="A4" s="3" t="inlineStr">
         <is>
           <t>Positive</t>
         </is>
       </c>
-      <c r="B4" s="0" t="n">
+      <c r="B4" s="3" t="n">
         <v>0.06</v>
       </c>
-      <c r="C4" s="0" t="n">
+      <c r="C4" s="3" t="n">
         <v>0.09</v>
       </c>
     </row>
     <row r="5">
-      <c r="A5" s="0" t="inlineStr">
+      <c r="A5" s="3" t="inlineStr">
         <is>
           <t>Neutral</t>
         </is>
       </c>
-      <c r="B5" s="0" t="n">
+      <c r="B5" s="3" t="n">
         <v>0.08</v>
       </c>
-      <c r="C5" s="0" t="n">
+      <c r="C5" s="3" t="n">
         <v>0.08</v>
       </c>
     </row>
     <row r="6">
-      <c r="A6" s="0" t="inlineStr">
+      <c r="A6" s="3" t="inlineStr">
         <is>
           <t>Negative</t>
         </is>
       </c>
-      <c r="B6" s="0" t="n">
+      <c r="B6" s="3" t="n">
         <v>0.86</v>
       </c>
-      <c r="C6" s="0" t="n">
+      <c r="C6" s="3" t="n">
         <v>0.83</v>
       </c>
     </row>
     <row r="7">
-      <c r="A7" s="0" t="inlineStr">
+      <c r="A7" s="4" t="inlineStr">
         <is>
           <t>Total</t>
         </is>
       </c>
-      <c r="B7" s="0" t="n">
+      <c r="B7" s="4" t="n">
         <v>87</v>
       </c>
-      <c r="C7" s="0" t="n">
+      <c r="C7" s="4" t="n">
         <v>174</v>
       </c>
     </row>
     <row r="8">
-      <c r="A8" s="0" t="inlineStr">
+      <c r="A8" s="4" t="inlineStr">
         <is>
           <t>Message Index</t>
         </is>
       </c>
-      <c r="B8" s="0" t="n">
+      <c r="B8" s="4" t="n">
         <v>93</v>
       </c>
-      <c r="C8" s="0" t="n">
+      <c r="C8" s="4" t="n">
         <v>186</v>
       </c>
     </row>
@@ -1423,6 +2475,410 @@
   <pageMargins right="0.75" left="0.75" bottom="1.0" top="1.0" footer="0.5" header="0.5"/>
   <pageSetup/>
   <headerFooter/>
-  <drawing r:id="rId30"/>
+  <drawing r:id="rId69"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xml:space="preserve">
+  <sheetPr>
+    <pageSetUpPr fitToPage="false"/>
+  </sheetPr>
+  <dimension ref="A1:C8"/>
+  <sheetViews>
+    <sheetView windowProtection="false" tabSelected="false" showWhiteSpace="false" showOutlineSymbols="false" showFormulas="false" rightToLeft="false" showZeros="true" showRuler="true" showRowColHeaders="true" showGridLines="true" defaultGridColor="true" zoomScale="100" workbookViewId="0" zoomScaleSheetLayoutView="0" zoomScalePageLayoutView="0" zoomScaleNormal="0"/>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="8" defaultRowHeight="18"/>
+  <cols>
+    <col min="1" max="1" bestFit="true" customWidth="true" width="14.534831460674157"/>
+    <col min="2" max="2" bestFit="true" customWidth="true" width="9.584831460674158"/>
+    <col min="3" max="3" bestFit="true" customWidth="true" width="9.584831460674158"/>
+  </cols>
+  <sheetData>
+    <row r="1">
+      <c r="A1" s="0" t="inlineStr">
+        <is>
+          <r>
+            <rPr>
+              <sz val="12"/>
+              <rFont val="Calibri"/>
+              <b val="true"/>
+            </rPr>
+            <t>Graphs</t>
+          </r>
+        </is>
+      </c>
+    </row>
+    <row r="2">
+      <c r="A2" s="0" t="inlineStr">
+        <is>
+          <r>
+            <rPr>
+              <sz val="12"/>
+              <rFont val="Calibri"/>
+              <b val="true"/>
+            </rPr>
+            <t>Mindset</t>
+          </r>
+        </is>
+      </c>
+    </row>
+    <row r="3">
+      <c r="A3" s="3" t="inlineStr">
+        <is>
+          <t/>
+        </is>
+      </c>
+      <c r="B3" s="3" t="inlineStr">
+        <is>
+          <t>T1</t>
+        </is>
+      </c>
+      <c r="C3" s="3" t="inlineStr">
+        <is>
+          <t> T2</t>
+        </is>
+      </c>
+    </row>
+    <row r="4">
+      <c r="A4" s="3" t="inlineStr">
+        <is>
+          <t>Unattracted</t>
+        </is>
+      </c>
+      <c r="B4" s="3" t="n">
+        <v>0.77</v>
+      </c>
+      <c r="C4" s="3" t="n">
+        <v>0.74</v>
+      </c>
+    </row>
+    <row r="5">
+      <c r="A5" s="3" t="inlineStr">
+        <is>
+          <t>Apathetic</t>
+        </is>
+      </c>
+      <c r="B5" s="3" t="n">
+        <v>0.18</v>
+      </c>
+      <c r="C5" s="3" t="n">
+        <v>0.17</v>
+      </c>
+    </row>
+    <row r="6">
+      <c r="A6" s="3" t="inlineStr">
+        <is>
+          <t>Attracted</t>
+        </is>
+      </c>
+      <c r="B6" s="3" t="n">
+        <v>0.03</v>
+      </c>
+      <c r="C6" s="3" t="n">
+        <v>0.06</v>
+      </c>
+    </row>
+    <row r="7">
+      <c r="A7" s="3" t="inlineStr">
+        <is>
+          <t>Impassioned</t>
+        </is>
+      </c>
+      <c r="B7" s="3" t="n">
+        <v>0.02</v>
+      </c>
+      <c r="C7" s="3" t="n">
+        <v>0.03</v>
+      </c>
+    </row>
+    <row r="8">
+      <c r="A8" s="4" t="inlineStr">
+        <is>
+          <t>Total</t>
+        </is>
+      </c>
+      <c r="B8" s="4" t="n">
+        <v>180</v>
+      </c>
+      <c r="C8" s="4" t="n">
+        <v>360</v>
+      </c>
+    </row>
+  </sheetData>
+  <sheetCalcPr fullCalcOnLoad="true"/>
+  <printOptions verticalCentered="false" horizontalCentered="false" headings="false" gridLines="false"/>
+  <pageMargins right="0.75" left="0.75" bottom="1.0" top="1.0" footer="0.5" header="0.5"/>
+  <pageSetup/>
+  <headerFooter/>
+  <drawing r:id="rId71"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xml:space="preserve">
+  <sheetPr>
+    <pageSetUpPr fitToPage="false"/>
+  </sheetPr>
+  <dimension ref="A1:C8"/>
+  <sheetViews>
+    <sheetView windowProtection="false" tabSelected="false" showWhiteSpace="false" showOutlineSymbols="false" showFormulas="false" rightToLeft="false" showZeros="true" showRuler="true" showRowColHeaders="true" showGridLines="true" defaultGridColor="true" zoomScale="100" workbookViewId="0" zoomScaleSheetLayoutView="0" zoomScalePageLayoutView="0" zoomScaleNormal="0"/>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="8" defaultRowHeight="18"/>
+  <cols>
+    <col min="1" max="1" bestFit="true" customWidth="true" width="26.170786516853934"/>
+    <col min="2" max="2" bestFit="true" customWidth="true" width="9.584831460674158"/>
+    <col min="3" max="3" bestFit="true" customWidth="true" width="9.584831460674158"/>
+  </cols>
+  <sheetData>
+    <row r="1">
+      <c r="A1" s="0" t="inlineStr">
+        <is>
+          <r>
+            <rPr>
+              <sz val="12"/>
+              <b val="true"/>
+            </rPr>
+            <t>Graphs</t>
+          </r>
+        </is>
+      </c>
+    </row>
+    <row r="2">
+      <c r="A2" s="0" t="inlineStr">
+        <is>
+          <r>
+            <rPr>
+              <sz val="12"/>
+              <b val="true"/>
+            </rPr>
+            <t>M1 NUEDEXTA User - Graphs</t>
+          </r>
+        </is>
+      </c>
+    </row>
+    <row r="3">
+      <c r="A3" s="3" t="inlineStr">
+        <is>
+          <t/>
+        </is>
+      </c>
+      <c r="B3" s="3" t="inlineStr">
+        <is>
+          <t>T1</t>
+        </is>
+      </c>
+      <c r="C3" s="3" t="inlineStr">
+        <is>
+          <t> T2</t>
+        </is>
+      </c>
+    </row>
+    <row r="4">
+      <c r="A4" s="3" t="inlineStr">
+        <is>
+          <t>Unattracted</t>
+        </is>
+      </c>
+      <c r="B4" s="3" t="n">
+        <v>0.69</v>
+      </c>
+      <c r="C4" s="3" t="n">
+        <v>0.67</v>
+      </c>
+    </row>
+    <row r="5">
+      <c r="A5" s="3" t="inlineStr">
+        <is>
+          <t>Apathetic</t>
+        </is>
+      </c>
+      <c r="B5" s="3" t="n">
+        <v>0.24</v>
+      </c>
+      <c r="C5" s="3" t="n">
+        <v>0.22</v>
+      </c>
+    </row>
+    <row r="6">
+      <c r="A6" s="3" t="inlineStr">
+        <is>
+          <t>Attracted</t>
+        </is>
+      </c>
+      <c r="B6" s="3" t="n">
+        <v>0.07</v>
+      </c>
+      <c r="C6" s="3" t="n">
+        <v>0.09</v>
+      </c>
+    </row>
+    <row r="7">
+      <c r="A7" s="3" t="inlineStr">
+        <is>
+          <t>Impassioned</t>
+        </is>
+      </c>
+      <c r="B7" s="3" t="n">
+        <v>0.0</v>
+      </c>
+      <c r="C7" s="3" t="n">
+        <v>0.02</v>
+      </c>
+    </row>
+    <row r="8">
+      <c r="A8" s="4" t="inlineStr">
+        <is>
+          <t>Total</t>
+        </is>
+      </c>
+      <c r="B8" s="4" t="n">
+        <v>87</v>
+      </c>
+      <c r="C8" s="4" t="n">
+        <v>174</v>
+      </c>
+    </row>
+  </sheetData>
+  <sheetCalcPr fullCalcOnLoad="true"/>
+  <printOptions verticalCentered="false" horizontalCentered="false" headings="false" gridLines="false"/>
+  <pageMargins right="0.75" left="0.75" bottom="1.0" top="1.0" footer="0.5" header="0.5"/>
+  <pageSetup/>
+  <headerFooter/>
+  <drawing r:id="rId73"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xml:space="preserve">
+  <sheetPr>
+    <pageSetUpPr fitToPage="false"/>
+  </sheetPr>
+  <dimension ref="A1:C8"/>
+  <sheetViews>
+    <sheetView windowProtection="false" tabSelected="false" showWhiteSpace="false" showOutlineSymbols="false" showFormulas="false" rightToLeft="false" showZeros="true" showRuler="true" showRowColHeaders="true" showGridLines="true" defaultGridColor="true" zoomScale="100" workbookViewId="0" zoomScaleSheetLayoutView="0" zoomScalePageLayoutView="0" zoomScaleNormal="0"/>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="8" defaultRowHeight="18"/>
+  <cols>
+    <col min="1" max="1" bestFit="true" customWidth="true" width="20.170786516853934"/>
+    <col min="2" max="2" bestFit="true" customWidth="true" width="9.584831460674158"/>
+    <col min="3" max="3" bestFit="true" customWidth="true" width="9.584831460674158"/>
+  </cols>
+  <sheetData>
+    <row r="1">
+      <c r="A1" s="0" t="inlineStr">
+        <is>
+          <r>
+            <rPr>
+              <sz val="12"/>
+              <b val="true"/>
+            </rPr>
+            <t>Graphs</t>
+          </r>
+        </is>
+      </c>
+    </row>
+    <row r="2">
+      <c r="A2" s="0" t="inlineStr">
+        <is>
+          <r>
+            <rPr>
+              <sz val="12"/>
+              <b val="true"/>
+            </rPr>
+            <t>M1 Non User - Graphs</t>
+          </r>
+        </is>
+      </c>
+    </row>
+    <row r="3">
+      <c r="A3" s="3" t="inlineStr">
+        <is>
+          <t/>
+        </is>
+      </c>
+      <c r="B3" s="3" t="inlineStr">
+        <is>
+          <t>T1</t>
+        </is>
+      </c>
+      <c r="C3" s="3" t="inlineStr">
+        <is>
+          <t> T2</t>
+        </is>
+      </c>
+    </row>
+    <row r="4">
+      <c r="A4" s="3" t="inlineStr">
+        <is>
+          <t>Unattracted</t>
+        </is>
+      </c>
+      <c r="B4" s="3" t="n">
+        <v>0.84</v>
+      </c>
+      <c r="C4" s="3" t="n">
+        <v>0.81</v>
+      </c>
+    </row>
+    <row r="5">
+      <c r="A5" s="3" t="inlineStr">
+        <is>
+          <t>Apathetic</t>
+        </is>
+      </c>
+      <c r="B5" s="3" t="n">
+        <v>0.13</v>
+      </c>
+      <c r="C5" s="3" t="n">
+        <v>0.11</v>
+      </c>
+    </row>
+    <row r="6">
+      <c r="A6" s="3" t="inlineStr">
+        <is>
+          <t>Attracted</t>
+        </is>
+      </c>
+      <c r="B6" s="3" t="n">
+        <v>0.0</v>
+      </c>
+      <c r="C6" s="3" t="n">
+        <v>0.03</v>
+      </c>
+    </row>
+    <row r="7">
+      <c r="A7" s="3" t="inlineStr">
+        <is>
+          <t>Impassioned</t>
+        </is>
+      </c>
+      <c r="B7" s="3" t="n">
+        <v>0.03</v>
+      </c>
+      <c r="C7" s="3" t="n">
+        <v>0.05</v>
+      </c>
+    </row>
+    <row r="8">
+      <c r="A8" s="4" t="inlineStr">
+        <is>
+          <t>Total</t>
+        </is>
+      </c>
+      <c r="B8" s="4" t="n">
+        <v>93</v>
+      </c>
+      <c r="C8" s="4" t="n">
+        <v>186</v>
+      </c>
+    </row>
+  </sheetData>
+  <sheetCalcPr fullCalcOnLoad="true"/>
+  <printOptions verticalCentered="false" horizontalCentered="false" headings="false" gridLines="false"/>
+  <pageMargins right="0.75" left="0.75" bottom="1.0" top="1.0" footer="0.5" header="0.5"/>
+  <pageSetup/>
+  <headerFooter/>
+  <drawing r:id="rId75"/>
 </worksheet>
 </file>
</xml_diff>